<commit_message>
2nd Generation RD Extracted
</commit_message>
<xml_diff>
--- a/Data/Logs/Collected.xlsx
+++ b/Data/Logs/Collected.xlsx
@@ -1,20 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/george/Dropbox/Mac/Desktop/Projects/Capstone/Langague-Analysis/Data/Logs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D35E1BD-EEEF-234F-A344-3717EF10F7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="211">
   <si>
     <t>2020</t>
   </si>
@@ -310,9 +327,6 @@
     <t>AUD</t>
   </si>
   <si>
-    <t>ZOOM</t>
-  </si>
-  <si>
     <t>SIRI</t>
   </si>
   <si>
@@ -607,9 +621,6 @@
     <t>0001067837</t>
   </si>
   <si>
-    <t>0000822708</t>
-  </si>
-  <si>
     <t>0000908937</t>
   </si>
   <si>
@@ -650,13 +661,16 @@
   </si>
   <si>
     <t>0001091907</t>
+  </si>
+  <si>
+    <t>ZM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -719,6 +733,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -765,7 +787,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -797,9 +819,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -831,6 +871,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1006,14 +1064,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1057,7 +1117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1098,10 +1158,10 @@
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1142,10 +1202,10 @@
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1186,10 +1246,10 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1230,10 +1290,10 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1274,10 +1334,10 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1318,10 +1378,10 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1362,10 +1422,10 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1406,10 +1466,10 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1450,10 +1510,10 @@
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1494,10 +1554,10 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -1538,10 +1598,10 @@
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1582,10 +1642,10 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -1626,10 +1686,10 @@
         <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1670,10 +1730,10 @@
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1714,10 +1774,10 @@
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -1758,10 +1818,10 @@
         <v>1</v>
       </c>
       <c r="N17" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1802,10 +1862,10 @@
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1846,10 +1906,10 @@
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -1890,10 +1950,10 @@
         <v>1</v>
       </c>
       <c r="N20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -1934,10 +1994,10 @@
         <v>1</v>
       </c>
       <c r="N21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -1978,10 +2038,10 @@
         <v>1</v>
       </c>
       <c r="N22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
@@ -2022,10 +2082,10 @@
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -2066,10 +2126,10 @@
         <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
@@ -2110,10 +2170,10 @@
         <v>0</v>
       </c>
       <c r="N25" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
@@ -2154,10 +2214,10 @@
         <v>1</v>
       </c>
       <c r="N26" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
@@ -2198,10 +2258,10 @@
         <v>1</v>
       </c>
       <c r="N27" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
@@ -2242,10 +2302,10 @@
         <v>1</v>
       </c>
       <c r="N28" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -2286,10 +2346,10 @@
         <v>1</v>
       </c>
       <c r="N29" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>42</v>
       </c>
@@ -2330,10 +2390,10 @@
         <v>1</v>
       </c>
       <c r="N30" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>43</v>
       </c>
@@ -2374,10 +2434,10 @@
         <v>1</v>
       </c>
       <c r="N31" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -2418,10 +2478,10 @@
         <v>1</v>
       </c>
       <c r="N32" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>45</v>
       </c>
@@ -2462,10 +2522,10 @@
         <v>1</v>
       </c>
       <c r="N33" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -2506,10 +2566,10 @@
         <v>1</v>
       </c>
       <c r="N34" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>47</v>
       </c>
@@ -2550,10 +2610,10 @@
         <v>1</v>
       </c>
       <c r="N35" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>48</v>
       </c>
@@ -2594,10 +2654,10 @@
         <v>1</v>
       </c>
       <c r="N36" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>49</v>
       </c>
@@ -2638,10 +2698,10 @@
         <v>1</v>
       </c>
       <c r="N37" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>50</v>
       </c>
@@ -2682,10 +2742,10 @@
         <v>1</v>
       </c>
       <c r="N38" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>51</v>
       </c>
@@ -2726,10 +2786,10 @@
         <v>1</v>
       </c>
       <c r="N39" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>52</v>
       </c>
@@ -2770,10 +2830,10 @@
         <v>1</v>
       </c>
       <c r="N40" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>53</v>
       </c>
@@ -2814,10 +2874,10 @@
         <v>1</v>
       </c>
       <c r="N41" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>54</v>
       </c>
@@ -2858,10 +2918,10 @@
         <v>1</v>
       </c>
       <c r="N42" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>55</v>
       </c>
@@ -2902,10 +2962,10 @@
         <v>1</v>
       </c>
       <c r="N43" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>56</v>
       </c>
@@ -2946,10 +3006,10 @@
         <v>1</v>
       </c>
       <c r="N44" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>57</v>
       </c>
@@ -2990,10 +3050,10 @@
         <v>1</v>
       </c>
       <c r="N45" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>58</v>
       </c>
@@ -3034,10 +3094,10 @@
         <v>1</v>
       </c>
       <c r="N46" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>59</v>
       </c>
@@ -3078,10 +3138,10 @@
         <v>1</v>
       </c>
       <c r="N47" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>60</v>
       </c>
@@ -3122,10 +3182,10 @@
         <v>1</v>
       </c>
       <c r="N48" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>61</v>
       </c>
@@ -3166,10 +3226,10 @@
         <v>1</v>
       </c>
       <c r="N49" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>62</v>
       </c>
@@ -3210,10 +3270,10 @@
         <v>1</v>
       </c>
       <c r="N50" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>63</v>
       </c>
@@ -3254,10 +3314,10 @@
         <v>1</v>
       </c>
       <c r="N51" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>64</v>
       </c>
@@ -3298,10 +3358,10 @@
         <v>1</v>
       </c>
       <c r="N52" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>65</v>
       </c>
@@ -3342,10 +3402,10 @@
         <v>1</v>
       </c>
       <c r="N53" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>66</v>
       </c>
@@ -3386,10 +3446,10 @@
         <v>1</v>
       </c>
       <c r="N54" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>67</v>
       </c>
@@ -3430,10 +3490,10 @@
         <v>1</v>
       </c>
       <c r="N55" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>68</v>
       </c>
@@ -3474,10 +3534,10 @@
         <v>1</v>
       </c>
       <c r="N56" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>69</v>
       </c>
@@ -3518,10 +3578,10 @@
         <v>1</v>
       </c>
       <c r="N57" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>70</v>
       </c>
@@ -3562,10 +3622,10 @@
         <v>1</v>
       </c>
       <c r="N58" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>71</v>
       </c>
@@ -3606,10 +3666,10 @@
         <v>1</v>
       </c>
       <c r="N59" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>72</v>
       </c>
@@ -3650,10 +3710,10 @@
         <v>1</v>
       </c>
       <c r="N60" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>73</v>
       </c>
@@ -3694,10 +3754,10 @@
         <v>1</v>
       </c>
       <c r="N61" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>74</v>
       </c>
@@ -3738,10 +3798,10 @@
         <v>1</v>
       </c>
       <c r="N62" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>75</v>
       </c>
@@ -3782,10 +3842,10 @@
         <v>1</v>
       </c>
       <c r="N63" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>76</v>
       </c>
@@ -3826,10 +3886,10 @@
         <v>1</v>
       </c>
       <c r="N64" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>77</v>
       </c>
@@ -3870,10 +3930,10 @@
         <v>1</v>
       </c>
       <c r="N65" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>78</v>
       </c>
@@ -3914,10 +3974,10 @@
         <v>1</v>
       </c>
       <c r="N66" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>79</v>
       </c>
@@ -3958,10 +4018,10 @@
         <v>1</v>
       </c>
       <c r="N67" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>80</v>
       </c>
@@ -4002,10 +4062,10 @@
         <v>1</v>
       </c>
       <c r="N68" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>81</v>
       </c>
@@ -4046,10 +4106,10 @@
         <v>1</v>
       </c>
       <c r="N69" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>82</v>
       </c>
@@ -4090,10 +4150,10 @@
         <v>1</v>
       </c>
       <c r="N70" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>83</v>
       </c>
@@ -4134,10 +4194,10 @@
         <v>1</v>
       </c>
       <c r="N71" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>84</v>
       </c>
@@ -4178,10 +4238,10 @@
         <v>1</v>
       </c>
       <c r="N72" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>85</v>
       </c>
@@ -4222,10 +4282,10 @@
         <v>1</v>
       </c>
       <c r="N73" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>86</v>
       </c>
@@ -4266,10 +4326,10 @@
         <v>1</v>
       </c>
       <c r="N74" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>87</v>
       </c>
@@ -4310,10 +4370,10 @@
         <v>1</v>
       </c>
       <c r="N75" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>88</v>
       </c>
@@ -4354,10 +4414,10 @@
         <v>1</v>
       </c>
       <c r="N76" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>89</v>
       </c>
@@ -4398,10 +4458,10 @@
         <v>1</v>
       </c>
       <c r="N77" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>90</v>
       </c>
@@ -4442,10 +4502,10 @@
         <v>0</v>
       </c>
       <c r="N78" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>91</v>
       </c>
@@ -4486,10 +4546,10 @@
         <v>0</v>
       </c>
       <c r="N79" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>92</v>
       </c>
@@ -4530,10 +4590,10 @@
         <v>0</v>
       </c>
       <c r="N80" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>93</v>
       </c>
@@ -4574,10 +4634,10 @@
         <v>0</v>
       </c>
       <c r="N81" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>94</v>
       </c>
@@ -4618,10 +4678,10 @@
         <v>0</v>
       </c>
       <c r="N82" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>95</v>
       </c>
@@ -4662,10 +4722,10 @@
         <v>0</v>
       </c>
       <c r="N83" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>96</v>
       </c>
@@ -4706,10 +4766,10 @@
         <v>0</v>
       </c>
       <c r="N84" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>97</v>
       </c>
@@ -4750,667 +4810,668 @@
         <v>0</v>
       </c>
       <c r="N85" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B86" t="b">
+        <v>0</v>
+      </c>
+      <c r="C86" t="b">
+        <v>0</v>
+      </c>
+      <c r="D86" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" t="b">
+        <v>0</v>
+      </c>
+      <c r="F86" t="b">
+        <v>0</v>
+      </c>
+      <c r="G86" t="b">
+        <v>0</v>
+      </c>
+      <c r="H86" t="b">
+        <v>0</v>
+      </c>
+      <c r="I86" t="b">
+        <v>0</v>
+      </c>
+      <c r="J86" t="b">
+        <v>0</v>
+      </c>
+      <c r="K86" t="b">
+        <v>0</v>
+      </c>
+      <c r="L86" t="b">
+        <v>0</v>
+      </c>
+      <c r="M86" t="b">
+        <v>0</v>
+      </c>
+      <c r="N86" t="str">
+        <f>"0001585521"</f>
+        <v>0001585521</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B87" t="b">
+        <v>0</v>
+      </c>
+      <c r="C87" t="b">
+        <v>0</v>
+      </c>
+      <c r="D87" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" t="b">
+        <v>0</v>
+      </c>
+      <c r="F87" t="b">
+        <v>0</v>
+      </c>
+      <c r="G87" t="b">
+        <v>0</v>
+      </c>
+      <c r="H87" t="b">
+        <v>0</v>
+      </c>
+      <c r="I87" t="b">
+        <v>0</v>
+      </c>
+      <c r="J87" t="b">
+        <v>0</v>
+      </c>
+      <c r="K87" t="b">
+        <v>0</v>
+      </c>
+      <c r="L87" t="b">
+        <v>0</v>
+      </c>
+      <c r="M87" t="b">
+        <v>0</v>
+      </c>
+      <c r="N87" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="86" spans="1:14">
-      <c r="A86" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B86" t="b">
-        <v>0</v>
-      </c>
-      <c r="C86" t="b">
-        <v>0</v>
-      </c>
-      <c r="D86" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" t="b">
-        <v>0</v>
-      </c>
-      <c r="F86" t="b">
-        <v>0</v>
-      </c>
-      <c r="G86" t="b">
-        <v>0</v>
-      </c>
-      <c r="H86" t="b">
-        <v>0</v>
-      </c>
-      <c r="I86" t="b">
-        <v>0</v>
-      </c>
-      <c r="J86" t="b">
-        <v>0</v>
-      </c>
-      <c r="K86" t="b">
-        <v>0</v>
-      </c>
-      <c r="L86" t="b">
-        <v>0</v>
-      </c>
-      <c r="M86" t="b">
-        <v>0</v>
-      </c>
-      <c r="N86" t="s">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B88" t="b">
+        <v>0</v>
+      </c>
+      <c r="C88" t="b">
+        <v>0</v>
+      </c>
+      <c r="D88" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" t="b">
+        <v>0</v>
+      </c>
+      <c r="F88" t="b">
+        <v>0</v>
+      </c>
+      <c r="G88" t="b">
+        <v>0</v>
+      </c>
+      <c r="H88" t="b">
+        <v>0</v>
+      </c>
+      <c r="I88" t="b">
+        <v>0</v>
+      </c>
+      <c r="J88" t="b">
+        <v>0</v>
+      </c>
+      <c r="K88" t="b">
+        <v>0</v>
+      </c>
+      <c r="L88" t="b">
+        <v>0</v>
+      </c>
+      <c r="M88" t="b">
+        <v>0</v>
+      </c>
+      <c r="N88" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="87" spans="1:14">
-      <c r="A87" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B87" t="b">
-        <v>0</v>
-      </c>
-      <c r="C87" t="b">
-        <v>0</v>
-      </c>
-      <c r="D87" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" t="b">
-        <v>0</v>
-      </c>
-      <c r="F87" t="b">
-        <v>0</v>
-      </c>
-      <c r="G87" t="b">
-        <v>0</v>
-      </c>
-      <c r="H87" t="b">
-        <v>0</v>
-      </c>
-      <c r="I87" t="b">
-        <v>0</v>
-      </c>
-      <c r="J87" t="b">
-        <v>0</v>
-      </c>
-      <c r="K87" t="b">
-        <v>0</v>
-      </c>
-      <c r="L87" t="b">
-        <v>0</v>
-      </c>
-      <c r="M87" t="b">
-        <v>0</v>
-      </c>
-      <c r="N87" t="s">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B89" t="b">
+        <v>0</v>
+      </c>
+      <c r="C89" t="b">
+        <v>0</v>
+      </c>
+      <c r="D89" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" t="b">
+        <v>0</v>
+      </c>
+      <c r="F89" t="b">
+        <v>0</v>
+      </c>
+      <c r="G89" t="b">
+        <v>0</v>
+      </c>
+      <c r="H89" t="b">
+        <v>0</v>
+      </c>
+      <c r="I89" t="b">
+        <v>0</v>
+      </c>
+      <c r="J89" t="b">
+        <v>0</v>
+      </c>
+      <c r="K89" t="b">
+        <v>0</v>
+      </c>
+      <c r="L89" t="b">
+        <v>0</v>
+      </c>
+      <c r="M89" t="b">
+        <v>0</v>
+      </c>
+      <c r="N89" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
-      <c r="A88" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B88" t="b">
-        <v>0</v>
-      </c>
-      <c r="C88" t="b">
-        <v>0</v>
-      </c>
-      <c r="D88" t="b">
-        <v>0</v>
-      </c>
-      <c r="E88" t="b">
-        <v>0</v>
-      </c>
-      <c r="F88" t="b">
-        <v>0</v>
-      </c>
-      <c r="G88" t="b">
-        <v>0</v>
-      </c>
-      <c r="H88" t="b">
-        <v>0</v>
-      </c>
-      <c r="I88" t="b">
-        <v>0</v>
-      </c>
-      <c r="J88" t="b">
-        <v>0</v>
-      </c>
-      <c r="K88" t="b">
-        <v>0</v>
-      </c>
-      <c r="L88" t="b">
-        <v>0</v>
-      </c>
-      <c r="M88" t="b">
-        <v>0</v>
-      </c>
-      <c r="N88" t="s">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90" t="b">
+        <v>0</v>
+      </c>
+      <c r="C90" t="b">
+        <v>0</v>
+      </c>
+      <c r="D90" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" t="b">
+        <v>0</v>
+      </c>
+      <c r="F90" t="b">
+        <v>0</v>
+      </c>
+      <c r="G90" t="b">
+        <v>0</v>
+      </c>
+      <c r="H90" t="b">
+        <v>0</v>
+      </c>
+      <c r="I90" t="b">
+        <v>0</v>
+      </c>
+      <c r="J90" t="b">
+        <v>0</v>
+      </c>
+      <c r="K90" t="b">
+        <v>0</v>
+      </c>
+      <c r="L90" t="b">
+        <v>0</v>
+      </c>
+      <c r="M90" t="b">
+        <v>0</v>
+      </c>
+      <c r="N90" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="89" spans="1:14">
-      <c r="A89" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B89" t="b">
-        <v>0</v>
-      </c>
-      <c r="C89" t="b">
-        <v>0</v>
-      </c>
-      <c r="D89" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" t="b">
-        <v>0</v>
-      </c>
-      <c r="F89" t="b">
-        <v>0</v>
-      </c>
-      <c r="G89" t="b">
-        <v>0</v>
-      </c>
-      <c r="H89" t="b">
-        <v>0</v>
-      </c>
-      <c r="I89" t="b">
-        <v>0</v>
-      </c>
-      <c r="J89" t="b">
-        <v>0</v>
-      </c>
-      <c r="K89" t="b">
-        <v>0</v>
-      </c>
-      <c r="L89" t="b">
-        <v>0</v>
-      </c>
-      <c r="M89" t="b">
-        <v>0</v>
-      </c>
-      <c r="N89" t="s">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B91" t="b">
+        <v>0</v>
+      </c>
+      <c r="C91" t="b">
+        <v>0</v>
+      </c>
+      <c r="D91" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" t="b">
+        <v>0</v>
+      </c>
+      <c r="F91" t="b">
+        <v>0</v>
+      </c>
+      <c r="G91" t="b">
+        <v>0</v>
+      </c>
+      <c r="H91" t="b">
+        <v>0</v>
+      </c>
+      <c r="I91" t="b">
+        <v>0</v>
+      </c>
+      <c r="J91" t="b">
+        <v>0</v>
+      </c>
+      <c r="K91" t="b">
+        <v>0</v>
+      </c>
+      <c r="L91" t="b">
+        <v>0</v>
+      </c>
+      <c r="M91" t="b">
+        <v>0</v>
+      </c>
+      <c r="N91" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="90" spans="1:14">
-      <c r="A90" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B90" t="b">
-        <v>0</v>
-      </c>
-      <c r="C90" t="b">
-        <v>0</v>
-      </c>
-      <c r="D90" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" t="b">
-        <v>0</v>
-      </c>
-      <c r="F90" t="b">
-        <v>0</v>
-      </c>
-      <c r="G90" t="b">
-        <v>0</v>
-      </c>
-      <c r="H90" t="b">
-        <v>0</v>
-      </c>
-      <c r="I90" t="b">
-        <v>0</v>
-      </c>
-      <c r="J90" t="b">
-        <v>0</v>
-      </c>
-      <c r="K90" t="b">
-        <v>0</v>
-      </c>
-      <c r="L90" t="b">
-        <v>0</v>
-      </c>
-      <c r="M90" t="b">
-        <v>0</v>
-      </c>
-      <c r="N90" t="s">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B92" t="b">
+        <v>0</v>
+      </c>
+      <c r="C92" t="b">
+        <v>0</v>
+      </c>
+      <c r="D92" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" t="b">
+        <v>0</v>
+      </c>
+      <c r="F92" t="b">
+        <v>0</v>
+      </c>
+      <c r="G92" t="b">
+        <v>0</v>
+      </c>
+      <c r="H92" t="b">
+        <v>0</v>
+      </c>
+      <c r="I92" t="b">
+        <v>0</v>
+      </c>
+      <c r="J92" t="b">
+        <v>0</v>
+      </c>
+      <c r="K92" t="b">
+        <v>0</v>
+      </c>
+      <c r="L92" t="b">
+        <v>0</v>
+      </c>
+      <c r="M92" t="b">
+        <v>0</v>
+      </c>
+      <c r="N92" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="91" spans="1:14">
-      <c r="A91" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B91" t="b">
-        <v>0</v>
-      </c>
-      <c r="C91" t="b">
-        <v>0</v>
-      </c>
-      <c r="D91" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" t="b">
-        <v>0</v>
-      </c>
-      <c r="F91" t="b">
-        <v>0</v>
-      </c>
-      <c r="G91" t="b">
-        <v>0</v>
-      </c>
-      <c r="H91" t="b">
-        <v>0</v>
-      </c>
-      <c r="I91" t="b">
-        <v>0</v>
-      </c>
-      <c r="J91" t="b">
-        <v>0</v>
-      </c>
-      <c r="K91" t="b">
-        <v>0</v>
-      </c>
-      <c r="L91" t="b">
-        <v>0</v>
-      </c>
-      <c r="M91" t="b">
-        <v>0</v>
-      </c>
-      <c r="N91" t="s">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B93" t="b">
+        <v>0</v>
+      </c>
+      <c r="C93" t="b">
+        <v>0</v>
+      </c>
+      <c r="D93" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" t="b">
+        <v>0</v>
+      </c>
+      <c r="F93" t="b">
+        <v>0</v>
+      </c>
+      <c r="G93" t="b">
+        <v>0</v>
+      </c>
+      <c r="H93" t="b">
+        <v>0</v>
+      </c>
+      <c r="I93" t="b">
+        <v>0</v>
+      </c>
+      <c r="J93" t="b">
+        <v>0</v>
+      </c>
+      <c r="K93" t="b">
+        <v>0</v>
+      </c>
+      <c r="L93" t="b">
+        <v>0</v>
+      </c>
+      <c r="M93" t="b">
+        <v>0</v>
+      </c>
+      <c r="N93" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="92" spans="1:14">
-      <c r="A92" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B92" t="b">
-        <v>0</v>
-      </c>
-      <c r="C92" t="b">
-        <v>0</v>
-      </c>
-      <c r="D92" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" t="b">
-        <v>0</v>
-      </c>
-      <c r="F92" t="b">
-        <v>0</v>
-      </c>
-      <c r="G92" t="b">
-        <v>0</v>
-      </c>
-      <c r="H92" t="b">
-        <v>0</v>
-      </c>
-      <c r="I92" t="b">
-        <v>0</v>
-      </c>
-      <c r="J92" t="b">
-        <v>0</v>
-      </c>
-      <c r="K92" t="b">
-        <v>0</v>
-      </c>
-      <c r="L92" t="b">
-        <v>0</v>
-      </c>
-      <c r="M92" t="b">
-        <v>0</v>
-      </c>
-      <c r="N92" t="s">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B94" t="b">
+        <v>0</v>
+      </c>
+      <c r="C94" t="b">
+        <v>0</v>
+      </c>
+      <c r="D94" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" t="b">
+        <v>0</v>
+      </c>
+      <c r="F94" t="b">
+        <v>0</v>
+      </c>
+      <c r="G94" t="b">
+        <v>0</v>
+      </c>
+      <c r="H94" t="b">
+        <v>0</v>
+      </c>
+      <c r="I94" t="b">
+        <v>0</v>
+      </c>
+      <c r="J94" t="b">
+        <v>0</v>
+      </c>
+      <c r="K94" t="b">
+        <v>0</v>
+      </c>
+      <c r="L94" t="b">
+        <v>0</v>
+      </c>
+      <c r="M94" t="b">
+        <v>0</v>
+      </c>
+      <c r="N94" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="93" spans="1:14">
-      <c r="A93" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B93" t="b">
-        <v>0</v>
-      </c>
-      <c r="C93" t="b">
-        <v>0</v>
-      </c>
-      <c r="D93" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" t="b">
-        <v>0</v>
-      </c>
-      <c r="F93" t="b">
-        <v>0</v>
-      </c>
-      <c r="G93" t="b">
-        <v>0</v>
-      </c>
-      <c r="H93" t="b">
-        <v>0</v>
-      </c>
-      <c r="I93" t="b">
-        <v>0</v>
-      </c>
-      <c r="J93" t="b">
-        <v>0</v>
-      </c>
-      <c r="K93" t="b">
-        <v>0</v>
-      </c>
-      <c r="L93" t="b">
-        <v>0</v>
-      </c>
-      <c r="M93" t="b">
-        <v>0</v>
-      </c>
-      <c r="N93" t="s">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B95" t="b">
+        <v>0</v>
+      </c>
+      <c r="C95" t="b">
+        <v>0</v>
+      </c>
+      <c r="D95" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" t="b">
+        <v>0</v>
+      </c>
+      <c r="F95" t="b">
+        <v>0</v>
+      </c>
+      <c r="G95" t="b">
+        <v>0</v>
+      </c>
+      <c r="H95" t="b">
+        <v>0</v>
+      </c>
+      <c r="I95" t="b">
+        <v>0</v>
+      </c>
+      <c r="J95" t="b">
+        <v>0</v>
+      </c>
+      <c r="K95" t="b">
+        <v>0</v>
+      </c>
+      <c r="L95" t="b">
+        <v>0</v>
+      </c>
+      <c r="M95" t="b">
+        <v>0</v>
+      </c>
+      <c r="N95" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="94" spans="1:14">
-      <c r="A94" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B94" t="b">
-        <v>0</v>
-      </c>
-      <c r="C94" t="b">
-        <v>0</v>
-      </c>
-      <c r="D94" t="b">
-        <v>0</v>
-      </c>
-      <c r="E94" t="b">
-        <v>0</v>
-      </c>
-      <c r="F94" t="b">
-        <v>0</v>
-      </c>
-      <c r="G94" t="b">
-        <v>0</v>
-      </c>
-      <c r="H94" t="b">
-        <v>0</v>
-      </c>
-      <c r="I94" t="b">
-        <v>0</v>
-      </c>
-      <c r="J94" t="b">
-        <v>0</v>
-      </c>
-      <c r="K94" t="b">
-        <v>0</v>
-      </c>
-      <c r="L94" t="b">
-        <v>0</v>
-      </c>
-      <c r="M94" t="b">
-        <v>0</v>
-      </c>
-      <c r="N94" t="s">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B96" t="b">
+        <v>0</v>
+      </c>
+      <c r="C96" t="b">
+        <v>0</v>
+      </c>
+      <c r="D96" t="b">
+        <v>0</v>
+      </c>
+      <c r="E96" t="b">
+        <v>0</v>
+      </c>
+      <c r="F96" t="b">
+        <v>0</v>
+      </c>
+      <c r="G96" t="b">
+        <v>0</v>
+      </c>
+      <c r="H96" t="b">
+        <v>0</v>
+      </c>
+      <c r="I96" t="b">
+        <v>0</v>
+      </c>
+      <c r="J96" t="b">
+        <v>0</v>
+      </c>
+      <c r="K96" t="b">
+        <v>0</v>
+      </c>
+      <c r="L96" t="b">
+        <v>0</v>
+      </c>
+      <c r="M96" t="b">
+        <v>0</v>
+      </c>
+      <c r="N96" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:14">
-      <c r="A95" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B95" t="b">
-        <v>0</v>
-      </c>
-      <c r="C95" t="b">
-        <v>0</v>
-      </c>
-      <c r="D95" t="b">
-        <v>0</v>
-      </c>
-      <c r="E95" t="b">
-        <v>0</v>
-      </c>
-      <c r="F95" t="b">
-        <v>0</v>
-      </c>
-      <c r="G95" t="b">
-        <v>0</v>
-      </c>
-      <c r="H95" t="b">
-        <v>0</v>
-      </c>
-      <c r="I95" t="b">
-        <v>0</v>
-      </c>
-      <c r="J95" t="b">
-        <v>0</v>
-      </c>
-      <c r="K95" t="b">
-        <v>0</v>
-      </c>
-      <c r="L95" t="b">
-        <v>0</v>
-      </c>
-      <c r="M95" t="b">
-        <v>0</v>
-      </c>
-      <c r="N95" t="s">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B97" t="b">
+        <v>0</v>
+      </c>
+      <c r="C97" t="b">
+        <v>0</v>
+      </c>
+      <c r="D97" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" t="b">
+        <v>0</v>
+      </c>
+      <c r="F97" t="b">
+        <v>0</v>
+      </c>
+      <c r="G97" t="b">
+        <v>0</v>
+      </c>
+      <c r="H97" t="b">
+        <v>0</v>
+      </c>
+      <c r="I97" t="b">
+        <v>0</v>
+      </c>
+      <c r="J97" t="b">
+        <v>0</v>
+      </c>
+      <c r="K97" t="b">
+        <v>0</v>
+      </c>
+      <c r="L97" t="b">
+        <v>0</v>
+      </c>
+      <c r="M97" t="b">
+        <v>0</v>
+      </c>
+      <c r="N97" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="96" spans="1:14">
-      <c r="A96" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B96" t="b">
-        <v>0</v>
-      </c>
-      <c r="C96" t="b">
-        <v>0</v>
-      </c>
-      <c r="D96" t="b">
-        <v>0</v>
-      </c>
-      <c r="E96" t="b">
-        <v>0</v>
-      </c>
-      <c r="F96" t="b">
-        <v>0</v>
-      </c>
-      <c r="G96" t="b">
-        <v>0</v>
-      </c>
-      <c r="H96" t="b">
-        <v>0</v>
-      </c>
-      <c r="I96" t="b">
-        <v>0</v>
-      </c>
-      <c r="J96" t="b">
-        <v>0</v>
-      </c>
-      <c r="K96" t="b">
-        <v>0</v>
-      </c>
-      <c r="L96" t="b">
-        <v>0</v>
-      </c>
-      <c r="M96" t="b">
-        <v>0</v>
-      </c>
-      <c r="N96" t="s">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B98" t="b">
+        <v>0</v>
+      </c>
+      <c r="C98" t="b">
+        <v>0</v>
+      </c>
+      <c r="D98" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98" t="b">
+        <v>0</v>
+      </c>
+      <c r="F98" t="b">
+        <v>0</v>
+      </c>
+      <c r="G98" t="b">
+        <v>0</v>
+      </c>
+      <c r="H98" t="b">
+        <v>0</v>
+      </c>
+      <c r="I98" t="b">
+        <v>0</v>
+      </c>
+      <c r="J98" t="b">
+        <v>0</v>
+      </c>
+      <c r="K98" t="b">
+        <v>0</v>
+      </c>
+      <c r="L98" t="b">
+        <v>0</v>
+      </c>
+      <c r="M98" t="b">
+        <v>0</v>
+      </c>
+      <c r="N98" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="97" spans="1:14">
-      <c r="A97" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B97" t="b">
-        <v>0</v>
-      </c>
-      <c r="C97" t="b">
-        <v>0</v>
-      </c>
-      <c r="D97" t="b">
-        <v>0</v>
-      </c>
-      <c r="E97" t="b">
-        <v>0</v>
-      </c>
-      <c r="F97" t="b">
-        <v>0</v>
-      </c>
-      <c r="G97" t="b">
-        <v>0</v>
-      </c>
-      <c r="H97" t="b">
-        <v>0</v>
-      </c>
-      <c r="I97" t="b">
-        <v>0</v>
-      </c>
-      <c r="J97" t="b">
-        <v>0</v>
-      </c>
-      <c r="K97" t="b">
-        <v>0</v>
-      </c>
-      <c r="L97" t="b">
-        <v>0</v>
-      </c>
-      <c r="M97" t="b">
-        <v>0</v>
-      </c>
-      <c r="N97" t="s">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B99" t="b">
+        <v>0</v>
+      </c>
+      <c r="C99" t="b">
+        <v>0</v>
+      </c>
+      <c r="D99" t="b">
+        <v>0</v>
+      </c>
+      <c r="E99" t="b">
+        <v>0</v>
+      </c>
+      <c r="F99" t="b">
+        <v>0</v>
+      </c>
+      <c r="G99" t="b">
+        <v>0</v>
+      </c>
+      <c r="H99" t="b">
+        <v>0</v>
+      </c>
+      <c r="I99" t="b">
+        <v>0</v>
+      </c>
+      <c r="J99" t="b">
+        <v>0</v>
+      </c>
+      <c r="K99" t="b">
+        <v>0</v>
+      </c>
+      <c r="L99" t="b">
+        <v>0</v>
+      </c>
+      <c r="M99" t="b">
+        <v>0</v>
+      </c>
+      <c r="N99" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="98" spans="1:14">
-      <c r="A98" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B98" t="b">
-        <v>0</v>
-      </c>
-      <c r="C98" t="b">
-        <v>0</v>
-      </c>
-      <c r="D98" t="b">
-        <v>0</v>
-      </c>
-      <c r="E98" t="b">
-        <v>0</v>
-      </c>
-      <c r="F98" t="b">
-        <v>0</v>
-      </c>
-      <c r="G98" t="b">
-        <v>0</v>
-      </c>
-      <c r="H98" t="b">
-        <v>0</v>
-      </c>
-      <c r="I98" t="b">
-        <v>0</v>
-      </c>
-      <c r="J98" t="b">
-        <v>0</v>
-      </c>
-      <c r="K98" t="b">
-        <v>0</v>
-      </c>
-      <c r="L98" t="b">
-        <v>0</v>
-      </c>
-      <c r="M98" t="b">
-        <v>0</v>
-      </c>
-      <c r="N98" t="s">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B100" t="b">
+        <v>0</v>
+      </c>
+      <c r="C100" t="b">
+        <v>0</v>
+      </c>
+      <c r="D100" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" t="b">
+        <v>0</v>
+      </c>
+      <c r="F100" t="b">
+        <v>0</v>
+      </c>
+      <c r="G100" t="b">
+        <v>0</v>
+      </c>
+      <c r="H100" t="b">
+        <v>0</v>
+      </c>
+      <c r="I100" t="b">
+        <v>0</v>
+      </c>
+      <c r="J100" t="b">
+        <v>0</v>
+      </c>
+      <c r="K100" t="b">
+        <v>0</v>
+      </c>
+      <c r="L100" t="b">
+        <v>0</v>
+      </c>
+      <c r="M100" t="b">
+        <v>0</v>
+      </c>
+      <c r="N100" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="99" spans="1:14">
-      <c r="A99" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B99" t="b">
-        <v>0</v>
-      </c>
-      <c r="C99" t="b">
-        <v>0</v>
-      </c>
-      <c r="D99" t="b">
-        <v>0</v>
-      </c>
-      <c r="E99" t="b">
-        <v>0</v>
-      </c>
-      <c r="F99" t="b">
-        <v>0</v>
-      </c>
-      <c r="G99" t="b">
-        <v>0</v>
-      </c>
-      <c r="H99" t="b">
-        <v>0</v>
-      </c>
-      <c r="I99" t="b">
-        <v>0</v>
-      </c>
-      <c r="J99" t="b">
-        <v>0</v>
-      </c>
-      <c r="K99" t="b">
-        <v>0</v>
-      </c>
-      <c r="L99" t="b">
-        <v>0</v>
-      </c>
-      <c r="M99" t="b">
-        <v>0</v>
-      </c>
-      <c r="N99" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="100" spans="1:14">
-      <c r="A100" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B100" t="b">
-        <v>0</v>
-      </c>
-      <c r="C100" t="b">
-        <v>0</v>
-      </c>
-      <c r="D100" t="b">
-        <v>0</v>
-      </c>
-      <c r="E100" t="b">
-        <v>0</v>
-      </c>
-      <c r="F100" t="b">
-        <v>0</v>
-      </c>
-      <c r="G100" t="b">
-        <v>0</v>
-      </c>
-      <c r="H100" t="b">
-        <v>0</v>
-      </c>
-      <c r="I100" t="b">
-        <v>0</v>
-      </c>
-      <c r="J100" t="b">
-        <v>0</v>
-      </c>
-      <c r="K100" t="b">
-        <v>0</v>
-      </c>
-      <c r="L100" t="b">
-        <v>0</v>
-      </c>
-      <c r="M100" t="b">
-        <v>0</v>
-      </c>
-      <c r="N100" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3rd Generation Universe Extraction
Attempt 5
</commit_message>
<xml_diff>
--- a/Data/Logs/Collected.xlsx
+++ b/Data/Logs/Collected.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="226">
   <si>
     <t>2020</t>
   </si>
@@ -124,9 +124,6 @@
     <t>DISH</t>
   </si>
   <si>
-    <t>DNB</t>
-  </si>
-  <si>
     <t>EA</t>
   </si>
   <si>
@@ -352,6 +349,33 @@
     <t>CMST</t>
   </si>
   <si>
+    <t>SFIX</t>
+  </si>
+  <si>
+    <t>CHWY</t>
+  </si>
+  <si>
+    <t>RNG</t>
+  </si>
+  <si>
+    <t>ETSY</t>
+  </si>
+  <si>
+    <t>PRTS</t>
+  </si>
+  <si>
+    <t>DASH</t>
+  </si>
+  <si>
+    <t>UBER</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>LYFT</t>
+  </si>
+  <si>
     <t>0001580808</t>
   </si>
   <si>
@@ -418,9 +442,6 @@
     <t>0001001082</t>
   </si>
   <si>
-    <t>0001799208</t>
-  </si>
-  <si>
     <t>0000712515</t>
   </si>
   <si>
@@ -644,6 +665,33 @@
   </si>
   <si>
     <t>0001166691</t>
+  </si>
+  <si>
+    <t>0001576942</t>
+  </si>
+  <si>
+    <t>0001766502</t>
+  </si>
+  <si>
+    <t>0001384905</t>
+  </si>
+  <si>
+    <t>0001370637</t>
+  </si>
+  <si>
+    <t>0001378950</t>
+  </si>
+  <si>
+    <t>0001792789</t>
+  </si>
+  <si>
+    <t>0001543151</t>
+  </si>
+  <si>
+    <t>0001810806</t>
+  </si>
+  <si>
+    <t>0001759509</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1049,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N99"/>
+  <dimension ref="A1:N107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1092,7 +1140,7 @@
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1136,7 +1184,7 @@
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1180,7 +1228,7 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -1224,7 +1272,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -1268,7 +1316,7 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1312,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -1356,7 +1404,7 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -1400,7 +1448,7 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -1444,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -1488,7 +1536,7 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1532,7 +1580,7 @@
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1576,7 +1624,7 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1620,7 +1668,7 @@
         <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -1664,7 +1712,7 @@
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1708,7 +1756,7 @@
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -1752,7 +1800,7 @@
         <v>1</v>
       </c>
       <c r="N17" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1796,7 +1844,7 @@
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1840,7 +1888,7 @@
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1884,7 +1932,7 @@
         <v>1</v>
       </c>
       <c r="N20" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1928,7 +1976,7 @@
         <v>1</v>
       </c>
       <c r="N21" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1972,7 +2020,7 @@
         <v>1</v>
       </c>
       <c r="N22" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -2016,7 +2064,7 @@
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -2024,31 +2072,31 @@
         <v>36</v>
       </c>
       <c r="B24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" t="b">
         <v>0</v>
@@ -2057,10 +2105,10 @@
         <v>0</v>
       </c>
       <c r="M24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -2089,10 +2137,10 @@
         <v>1</v>
       </c>
       <c r="I25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" t="b">
         <v>0</v>
@@ -2104,7 +2152,7 @@
         <v>1</v>
       </c>
       <c r="N25" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -2130,7 +2178,7 @@
         <v>1</v>
       </c>
       <c r="H26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" t="b">
         <v>0</v>
@@ -2148,7 +2196,7 @@
         <v>1</v>
       </c>
       <c r="N26" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -2171,7 +2219,7 @@
         <v>1</v>
       </c>
       <c r="G27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" t="b">
         <v>0</v>
@@ -2192,7 +2240,7 @@
         <v>1</v>
       </c>
       <c r="N27" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -2215,16 +2263,16 @@
         <v>1</v>
       </c>
       <c r="G28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" t="b">
         <v>0</v>
@@ -2236,7 +2284,7 @@
         <v>1</v>
       </c>
       <c r="N28" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -2250,25 +2298,25 @@
         <v>1</v>
       </c>
       <c r="D29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29" t="b">
         <v>0</v>
@@ -2280,7 +2328,7 @@
         <v>1</v>
       </c>
       <c r="N29" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -2294,19 +2342,19 @@
         <v>1</v>
       </c>
       <c r="D30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" t="b">
         <v>0</v>
@@ -2324,7 +2372,7 @@
         <v>1</v>
       </c>
       <c r="N30" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -2347,10 +2395,10 @@
         <v>1</v>
       </c>
       <c r="G31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" t="b">
         <v>0</v>
@@ -2368,7 +2416,7 @@
         <v>1</v>
       </c>
       <c r="N31" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -2382,13 +2430,13 @@
         <v>1</v>
       </c>
       <c r="D32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" t="b">
         <v>0</v>
@@ -2412,7 +2460,7 @@
         <v>1</v>
       </c>
       <c r="N32" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -2426,22 +2474,22 @@
         <v>1</v>
       </c>
       <c r="D33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" t="b">
         <v>0</v>
@@ -2456,7 +2504,7 @@
         <v>1</v>
       </c>
       <c r="N33" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -2473,7 +2521,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" t="b">
         <v>1</v>
@@ -2482,10 +2530,10 @@
         <v>1</v>
       </c>
       <c r="H34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="b">
         <v>0</v>
@@ -2500,7 +2548,7 @@
         <v>1</v>
       </c>
       <c r="N34" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -2517,13 +2565,13 @@
         <v>1</v>
       </c>
       <c r="E35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" t="b">
         <v>1</v>
       </c>
       <c r="G35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
@@ -2544,7 +2592,7 @@
         <v>1</v>
       </c>
       <c r="N35" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -2579,7 +2627,7 @@
         <v>0</v>
       </c>
       <c r="K36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L36" t="b">
         <v>0</v>
@@ -2588,7 +2636,7 @@
         <v>1</v>
       </c>
       <c r="N36" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -2611,16 +2659,16 @@
         <v>1</v>
       </c>
       <c r="G37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" t="b">
         <v>1</v>
@@ -2632,7 +2680,7 @@
         <v>1</v>
       </c>
       <c r="N37" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -2643,13 +2691,13 @@
         <v>1</v>
       </c>
       <c r="C38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" t="b">
         <v>1</v>
@@ -2664,10 +2712,10 @@
         <v>1</v>
       </c>
       <c r="J38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L38" t="b">
         <v>0</v>
@@ -2676,7 +2724,7 @@
         <v>1</v>
       </c>
       <c r="N38" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -2687,13 +2735,13 @@
         <v>1</v>
       </c>
       <c r="C39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" t="b">
         <v>1</v>
@@ -2708,10 +2756,10 @@
         <v>1</v>
       </c>
       <c r="J39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L39" t="b">
         <v>0</v>
@@ -2720,7 +2768,7 @@
         <v>1</v>
       </c>
       <c r="N39" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -2743,19 +2791,19 @@
         <v>1</v>
       </c>
       <c r="G40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L40" t="b">
         <v>0</v>
@@ -2764,7 +2812,7 @@
         <v>1</v>
       </c>
       <c r="N40" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -2787,13 +2835,13 @@
         <v>1</v>
       </c>
       <c r="G41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="b">
         <v>0</v>
@@ -2808,7 +2856,7 @@
         <v>1</v>
       </c>
       <c r="N41" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -2840,10 +2888,10 @@
         <v>1</v>
       </c>
       <c r="J42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L42" t="b">
         <v>0</v>
@@ -2852,7 +2900,7 @@
         <v>1</v>
       </c>
       <c r="N42" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -2872,22 +2920,22 @@
         <v>1</v>
       </c>
       <c r="F43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L43" t="b">
         <v>0</v>
@@ -2896,7 +2944,7 @@
         <v>1</v>
       </c>
       <c r="N43" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -2940,7 +2988,7 @@
         <v>1</v>
       </c>
       <c r="N44" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -2960,19 +3008,19 @@
         <v>1</v>
       </c>
       <c r="F45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K45" t="b">
         <v>0</v>
@@ -2984,7 +3032,7 @@
         <v>1</v>
       </c>
       <c r="N45" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:14">
@@ -3013,10 +3061,10 @@
         <v>1</v>
       </c>
       <c r="I46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K46" t="b">
         <v>0</v>
@@ -3028,7 +3076,7 @@
         <v>1</v>
       </c>
       <c r="N46" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -3057,10 +3105,10 @@
         <v>1</v>
       </c>
       <c r="I47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47" t="b">
         <v>0</v>
@@ -3072,7 +3120,7 @@
         <v>1</v>
       </c>
       <c r="N47" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:14">
@@ -3107,7 +3155,7 @@
         <v>1</v>
       </c>
       <c r="K48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L48" t="b">
         <v>0</v>
@@ -3116,7 +3164,7 @@
         <v>1</v>
       </c>
       <c r="N48" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:14">
@@ -3160,7 +3208,7 @@
         <v>1</v>
       </c>
       <c r="N49" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" spans="1:14">
@@ -3177,25 +3225,25 @@
         <v>1</v>
       </c>
       <c r="E50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L50" t="b">
         <v>0</v>
@@ -3204,7 +3252,7 @@
         <v>1</v>
       </c>
       <c r="N50" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:14">
@@ -3221,13 +3269,13 @@
         <v>1</v>
       </c>
       <c r="E51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" t="b">
         <v>0</v>
@@ -3248,7 +3296,7 @@
         <v>1</v>
       </c>
       <c r="N51" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:14">
@@ -3292,7 +3340,7 @@
         <v>1</v>
       </c>
       <c r="N52" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:14">
@@ -3318,7 +3366,7 @@
         <v>1</v>
       </c>
       <c r="H53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" t="b">
         <v>0</v>
@@ -3336,7 +3384,7 @@
         <v>1</v>
       </c>
       <c r="N53" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:14">
@@ -3365,13 +3413,13 @@
         <v>1</v>
       </c>
       <c r="I54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L54" t="b">
         <v>0</v>
@@ -3380,7 +3428,7 @@
         <v>1</v>
       </c>
       <c r="N54" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="1:14">
@@ -3409,13 +3457,13 @@
         <v>1</v>
       </c>
       <c r="I55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L55" t="b">
         <v>0</v>
@@ -3424,7 +3472,7 @@
         <v>1</v>
       </c>
       <c r="N55" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:14">
@@ -3468,7 +3516,7 @@
         <v>1</v>
       </c>
       <c r="N56" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:14">
@@ -3512,7 +3560,7 @@
         <v>1</v>
       </c>
       <c r="N57" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:14">
@@ -3520,25 +3568,25 @@
         <v>70</v>
       </c>
       <c r="B58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58" t="b">
         <v>0</v>
@@ -3556,7 +3604,7 @@
         <v>1</v>
       </c>
       <c r="N58" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:14">
@@ -3564,31 +3612,31 @@
         <v>71</v>
       </c>
       <c r="B59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K59" t="b">
         <v>0</v>
@@ -3600,7 +3648,7 @@
         <v>1</v>
       </c>
       <c r="N59" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:14">
@@ -3626,13 +3674,13 @@
         <v>1</v>
       </c>
       <c r="H60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K60" t="b">
         <v>0</v>
@@ -3644,7 +3692,7 @@
         <v>1</v>
       </c>
       <c r="N60" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
     </row>
     <row r="61" spans="1:14">
@@ -3688,7 +3736,7 @@
         <v>1</v>
       </c>
       <c r="N61" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62" spans="1:14">
@@ -3705,13 +3753,13 @@
         <v>1</v>
       </c>
       <c r="E62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62" t="b">
         <v>0</v>
@@ -3732,7 +3780,7 @@
         <v>1</v>
       </c>
       <c r="N62" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
     </row>
     <row r="63" spans="1:14">
@@ -3749,16 +3797,16 @@
         <v>1</v>
       </c>
       <c r="E63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I63" t="b">
         <v>0</v>
@@ -3776,7 +3824,7 @@
         <v>1</v>
       </c>
       <c r="N63" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:14">
@@ -3805,13 +3853,13 @@
         <v>1</v>
       </c>
       <c r="I64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L64" t="b">
         <v>0</v>
@@ -3820,7 +3868,7 @@
         <v>1</v>
       </c>
       <c r="N64" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
     <row r="65" spans="1:14">
@@ -3846,16 +3894,16 @@
         <v>1</v>
       </c>
       <c r="H65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L65" t="b">
         <v>0</v>
@@ -3864,7 +3912,7 @@
         <v>1</v>
       </c>
       <c r="N65" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="66" spans="1:14">
@@ -3890,16 +3938,16 @@
         <v>1</v>
       </c>
       <c r="H66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L66" t="b">
         <v>0</v>
@@ -3908,7 +3956,7 @@
         <v>1</v>
       </c>
       <c r="N66" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
     </row>
     <row r="67" spans="1:14">
@@ -3931,19 +3979,19 @@
         <v>1</v>
       </c>
       <c r="G67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L67" t="b">
         <v>0</v>
@@ -3952,7 +4000,7 @@
         <v>1</v>
       </c>
       <c r="N67" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
     <row r="68" spans="1:14">
@@ -3975,13 +4023,13 @@
         <v>1</v>
       </c>
       <c r="G68" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H68" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I68" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J68" t="b">
         <v>0</v>
@@ -3996,7 +4044,7 @@
         <v>1</v>
       </c>
       <c r="N68" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
     </row>
     <row r="69" spans="1:14">
@@ -4025,7 +4073,7 @@
         <v>1</v>
       </c>
       <c r="I69" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J69" t="b">
         <v>0</v>
@@ -4040,7 +4088,7 @@
         <v>1</v>
       </c>
       <c r="N69" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:14">
@@ -4069,10 +4117,10 @@
         <v>1</v>
       </c>
       <c r="I70" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J70" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K70" t="b">
         <v>0</v>
@@ -4084,7 +4132,7 @@
         <v>1</v>
       </c>
       <c r="N70" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:14">
@@ -4128,7 +4176,7 @@
         <v>1</v>
       </c>
       <c r="N71" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" spans="1:14">
@@ -4145,16 +4193,16 @@
         <v>1</v>
       </c>
       <c r="E72" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F72" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G72" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H72" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I72" t="b">
         <v>1</v>
@@ -4163,7 +4211,7 @@
         <v>1</v>
       </c>
       <c r="K72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L72" t="b">
         <v>0</v>
@@ -4172,7 +4220,7 @@
         <v>1</v>
       </c>
       <c r="N72" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
     <row r="73" spans="1:14">
@@ -4189,25 +4237,25 @@
         <v>1</v>
       </c>
       <c r="E73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I73" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J73" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K73" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L73" t="b">
         <v>0</v>
@@ -4216,7 +4264,7 @@
         <v>1</v>
       </c>
       <c r="N73" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="74" spans="1:14">
@@ -4239,10 +4287,10 @@
         <v>1</v>
       </c>
       <c r="G74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I74" t="b">
         <v>0</v>
@@ -4260,7 +4308,7 @@
         <v>1</v>
       </c>
       <c r="N74" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
     </row>
     <row r="75" spans="1:14">
@@ -4277,10 +4325,10 @@
         <v>1</v>
       </c>
       <c r="E75" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F75" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G75" t="b">
         <v>0</v>
@@ -4304,7 +4352,7 @@
         <v>1</v>
       </c>
       <c r="N75" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="76" spans="1:14">
@@ -4321,19 +4369,19 @@
         <v>1</v>
       </c>
       <c r="E76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J76" t="b">
         <v>0</v>
@@ -4348,7 +4396,7 @@
         <v>1</v>
       </c>
       <c r="N76" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="77" spans="1:14">
@@ -4371,13 +4419,13 @@
         <v>1</v>
       </c>
       <c r="G77" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H77" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I77" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J77" t="b">
         <v>0</v>
@@ -4392,7 +4440,7 @@
         <v>1</v>
       </c>
       <c r="N77" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="78" spans="1:14">
@@ -4415,19 +4463,19 @@
         <v>1</v>
       </c>
       <c r="G78" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H78" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I78" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J78" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K78" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L78" t="b">
         <v>0</v>
@@ -4436,7 +4484,7 @@
         <v>1</v>
       </c>
       <c r="N78" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
     </row>
     <row r="79" spans="1:14">
@@ -4453,25 +4501,25 @@
         <v>1</v>
       </c>
       <c r="E79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L79" t="b">
         <v>0</v>
@@ -4480,7 +4528,7 @@
         <v>1</v>
       </c>
       <c r="N79" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
     </row>
     <row r="80" spans="1:14">
@@ -4497,16 +4545,16 @@
         <v>1</v>
       </c>
       <c r="E80" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F80" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G80" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H80" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I80" t="b">
         <v>0</v>
@@ -4524,7 +4572,7 @@
         <v>1</v>
       </c>
       <c r="N80" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row r="81" spans="1:14">
@@ -4538,19 +4586,19 @@
         <v>1</v>
       </c>
       <c r="D81" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F81" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G81" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I81" t="b">
         <v>0</v>
@@ -4568,7 +4616,7 @@
         <v>1</v>
       </c>
       <c r="N81" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="82" spans="1:14">
@@ -4582,13 +4630,13 @@
         <v>1</v>
       </c>
       <c r="D82" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E82" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F82" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G82" t="b">
         <v>0</v>
@@ -4612,7 +4660,7 @@
         <v>1</v>
       </c>
       <c r="N82" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
     </row>
     <row r="83" spans="1:14">
@@ -4626,13 +4674,13 @@
         <v>1</v>
       </c>
       <c r="D83" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E83" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F83" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G83" t="b">
         <v>0</v>
@@ -4656,7 +4704,7 @@
         <v>1</v>
       </c>
       <c r="N83" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
     </row>
     <row r="84" spans="1:14">
@@ -4700,7 +4748,7 @@
         <v>1</v>
       </c>
       <c r="N84" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
     </row>
     <row r="85" spans="1:14">
@@ -4714,25 +4762,25 @@
         <v>1</v>
       </c>
       <c r="D85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K85" t="b">
         <v>0</v>
@@ -4744,7 +4792,7 @@
         <v>1</v>
       </c>
       <c r="N85" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row r="86" spans="1:14">
@@ -4779,7 +4827,7 @@
         <v>1</v>
       </c>
       <c r="K86" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L86" t="b">
         <v>0</v>
@@ -4788,7 +4836,7 @@
         <v>1</v>
       </c>
       <c r="N86" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
     </row>
     <row r="87" spans="1:14">
@@ -4811,19 +4859,19 @@
         <v>1</v>
       </c>
       <c r="G87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L87" t="b">
         <v>0</v>
@@ -4832,7 +4880,7 @@
         <v>1</v>
       </c>
       <c r="N87" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
     </row>
     <row r="88" spans="1:14">
@@ -4849,10 +4897,10 @@
         <v>1</v>
       </c>
       <c r="E88" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F88" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G88" t="b">
         <v>0</v>
@@ -4876,7 +4924,7 @@
         <v>1</v>
       </c>
       <c r="N88" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
     </row>
     <row r="89" spans="1:14">
@@ -4893,22 +4941,22 @@
         <v>1</v>
       </c>
       <c r="E89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K89" t="b">
         <v>0</v>
@@ -4920,7 +4968,7 @@
         <v>1</v>
       </c>
       <c r="N89" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
     </row>
     <row r="90" spans="1:14">
@@ -4928,31 +4976,31 @@
         <v>102</v>
       </c>
       <c r="B90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K90" t="b">
         <v>0</v>
@@ -4964,7 +5012,7 @@
         <v>1</v>
       </c>
       <c r="N90" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
     </row>
     <row r="91" spans="1:14">
@@ -4972,16 +5020,16 @@
         <v>103</v>
       </c>
       <c r="B91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F91" t="b">
         <v>0</v>
@@ -5008,7 +5056,7 @@
         <v>1</v>
       </c>
       <c r="N91" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
     <row r="92" spans="1:14">
@@ -5028,22 +5076,22 @@
         <v>1</v>
       </c>
       <c r="F92" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G92" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H92" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I92" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J92" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K92" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L92" t="b">
         <v>0</v>
@@ -5052,7 +5100,7 @@
         <v>1</v>
       </c>
       <c r="N92" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="93" spans="1:14">
@@ -5096,7 +5144,7 @@
         <v>1</v>
       </c>
       <c r="N93" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row r="94" spans="1:14">
@@ -5140,7 +5188,7 @@
         <v>1</v>
       </c>
       <c r="N94" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="95" spans="1:14">
@@ -5148,7 +5196,7 @@
         <v>107</v>
       </c>
       <c r="B95" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C95" t="b">
         <v>1</v>
@@ -5175,7 +5223,7 @@
         <v>1</v>
       </c>
       <c r="K95" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L95" t="b">
         <v>0</v>
@@ -5184,7 +5232,7 @@
         <v>1</v>
       </c>
       <c r="N95" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
     </row>
     <row r="96" spans="1:14">
@@ -5195,28 +5243,28 @@
         <v>0</v>
       </c>
       <c r="C96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K96" t="b">
         <v>0</v>
@@ -5228,7 +5276,7 @@
         <v>1</v>
       </c>
       <c r="N96" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
     </row>
     <row r="97" spans="1:14">
@@ -5242,25 +5290,25 @@
         <v>0</v>
       </c>
       <c r="D97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K97" t="b">
         <v>0</v>
@@ -5272,7 +5320,7 @@
         <v>1</v>
       </c>
       <c r="N97" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
     </row>
     <row r="98" spans="1:14">
@@ -5280,10 +5328,10 @@
         <v>110</v>
       </c>
       <c r="B98" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C98" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D98" t="b">
         <v>1</v>
@@ -5292,19 +5340,19 @@
         <v>1</v>
       </c>
       <c r="F98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K98" t="b">
         <v>0</v>
@@ -5316,7 +5364,7 @@
         <v>1</v>
       </c>
       <c r="N98" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="99" spans="1:14">
@@ -5324,16 +5372,16 @@
         <v>111</v>
       </c>
       <c r="B99" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C99" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D99" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F99" t="b">
         <v>0</v>
@@ -5357,10 +5405,362 @@
         <v>0</v>
       </c>
       <c r="M99" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N99" t="s">
-        <v>209</v>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14">
+      <c r="A100" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B100" t="b">
+        <v>0</v>
+      </c>
+      <c r="C100" t="b">
+        <v>0</v>
+      </c>
+      <c r="D100" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" t="b">
+        <v>0</v>
+      </c>
+      <c r="F100" t="b">
+        <v>0</v>
+      </c>
+      <c r="G100" t="b">
+        <v>0</v>
+      </c>
+      <c r="H100" t="b">
+        <v>0</v>
+      </c>
+      <c r="I100" t="b">
+        <v>0</v>
+      </c>
+      <c r="J100" t="b">
+        <v>0</v>
+      </c>
+      <c r="K100" t="b">
+        <v>0</v>
+      </c>
+      <c r="L100" t="b">
+        <v>0</v>
+      </c>
+      <c r="M100" t="b">
+        <v>0</v>
+      </c>
+      <c r="N100" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14">
+      <c r="A101" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B101" t="b">
+        <v>0</v>
+      </c>
+      <c r="C101" t="b">
+        <v>0</v>
+      </c>
+      <c r="D101" t="b">
+        <v>0</v>
+      </c>
+      <c r="E101" t="b">
+        <v>0</v>
+      </c>
+      <c r="F101" t="b">
+        <v>0</v>
+      </c>
+      <c r="G101" t="b">
+        <v>0</v>
+      </c>
+      <c r="H101" t="b">
+        <v>0</v>
+      </c>
+      <c r="I101" t="b">
+        <v>0</v>
+      </c>
+      <c r="J101" t="b">
+        <v>0</v>
+      </c>
+      <c r="K101" t="b">
+        <v>0</v>
+      </c>
+      <c r="L101" t="b">
+        <v>0</v>
+      </c>
+      <c r="M101" t="b">
+        <v>0</v>
+      </c>
+      <c r="N101" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14">
+      <c r="A102" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B102" t="b">
+        <v>0</v>
+      </c>
+      <c r="C102" t="b">
+        <v>0</v>
+      </c>
+      <c r="D102" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102" t="b">
+        <v>0</v>
+      </c>
+      <c r="F102" t="b">
+        <v>0</v>
+      </c>
+      <c r="G102" t="b">
+        <v>0</v>
+      </c>
+      <c r="H102" t="b">
+        <v>0</v>
+      </c>
+      <c r="I102" t="b">
+        <v>0</v>
+      </c>
+      <c r="J102" t="b">
+        <v>0</v>
+      </c>
+      <c r="K102" t="b">
+        <v>0</v>
+      </c>
+      <c r="L102" t="b">
+        <v>0</v>
+      </c>
+      <c r="M102" t="b">
+        <v>0</v>
+      </c>
+      <c r="N102" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14">
+      <c r="A103" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B103" t="b">
+        <v>0</v>
+      </c>
+      <c r="C103" t="b">
+        <v>0</v>
+      </c>
+      <c r="D103" t="b">
+        <v>0</v>
+      </c>
+      <c r="E103" t="b">
+        <v>0</v>
+      </c>
+      <c r="F103" t="b">
+        <v>0</v>
+      </c>
+      <c r="G103" t="b">
+        <v>0</v>
+      </c>
+      <c r="H103" t="b">
+        <v>0</v>
+      </c>
+      <c r="I103" t="b">
+        <v>0</v>
+      </c>
+      <c r="J103" t="b">
+        <v>0</v>
+      </c>
+      <c r="K103" t="b">
+        <v>0</v>
+      </c>
+      <c r="L103" t="b">
+        <v>0</v>
+      </c>
+      <c r="M103" t="b">
+        <v>0</v>
+      </c>
+      <c r="N103" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14">
+      <c r="A104" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B104" t="b">
+        <v>0</v>
+      </c>
+      <c r="C104" t="b">
+        <v>0</v>
+      </c>
+      <c r="D104" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104" t="b">
+        <v>0</v>
+      </c>
+      <c r="F104" t="b">
+        <v>0</v>
+      </c>
+      <c r="G104" t="b">
+        <v>0</v>
+      </c>
+      <c r="H104" t="b">
+        <v>0</v>
+      </c>
+      <c r="I104" t="b">
+        <v>0</v>
+      </c>
+      <c r="J104" t="b">
+        <v>0</v>
+      </c>
+      <c r="K104" t="b">
+        <v>0</v>
+      </c>
+      <c r="L104" t="b">
+        <v>0</v>
+      </c>
+      <c r="M104" t="b">
+        <v>0</v>
+      </c>
+      <c r="N104" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14">
+      <c r="A105" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B105" t="b">
+        <v>0</v>
+      </c>
+      <c r="C105" t="b">
+        <v>0</v>
+      </c>
+      <c r="D105" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105" t="b">
+        <v>0</v>
+      </c>
+      <c r="F105" t="b">
+        <v>0</v>
+      </c>
+      <c r="G105" t="b">
+        <v>0</v>
+      </c>
+      <c r="H105" t="b">
+        <v>0</v>
+      </c>
+      <c r="I105" t="b">
+        <v>0</v>
+      </c>
+      <c r="J105" t="b">
+        <v>0</v>
+      </c>
+      <c r="K105" t="b">
+        <v>0</v>
+      </c>
+      <c r="L105" t="b">
+        <v>0</v>
+      </c>
+      <c r="M105" t="b">
+        <v>0</v>
+      </c>
+      <c r="N105" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14">
+      <c r="A106" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B106" t="b">
+        <v>0</v>
+      </c>
+      <c r="C106" t="b">
+        <v>0</v>
+      </c>
+      <c r="D106" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106" t="b">
+        <v>0</v>
+      </c>
+      <c r="F106" t="b">
+        <v>0</v>
+      </c>
+      <c r="G106" t="b">
+        <v>0</v>
+      </c>
+      <c r="H106" t="b">
+        <v>0</v>
+      </c>
+      <c r="I106" t="b">
+        <v>0</v>
+      </c>
+      <c r="J106" t="b">
+        <v>0</v>
+      </c>
+      <c r="K106" t="b">
+        <v>0</v>
+      </c>
+      <c r="L106" t="b">
+        <v>0</v>
+      </c>
+      <c r="M106" t="b">
+        <v>0</v>
+      </c>
+      <c r="N106" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14">
+      <c r="A107" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B107" t="b">
+        <v>0</v>
+      </c>
+      <c r="C107" t="b">
+        <v>0</v>
+      </c>
+      <c r="D107" t="b">
+        <v>0</v>
+      </c>
+      <c r="E107" t="b">
+        <v>0</v>
+      </c>
+      <c r="F107" t="b">
+        <v>0</v>
+      </c>
+      <c r="G107" t="b">
+        <v>0</v>
+      </c>
+      <c r="H107" t="b">
+        <v>0</v>
+      </c>
+      <c r="I107" t="b">
+        <v>0</v>
+      </c>
+      <c r="J107" t="b">
+        <v>0</v>
+      </c>
+      <c r="K107" t="b">
+        <v>0</v>
+      </c>
+      <c r="L107" t="b">
+        <v>0</v>
+      </c>
+      <c r="M107" t="b">
+        <v>0</v>
+      </c>
+      <c r="N107" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue with Description Code
Fixed & Collected Remaining Stocks
</commit_message>
<xml_diff>
--- a/Data/Logs/Collected.xlsx
+++ b/Data/Logs/Collected.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/george/Dropbox/Mac/Desktop/Projects/Capstone/Langague-Analysis/Data/Logs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A345FC70-1E89-F345-9B3E-3F2D1F387D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -346,9 +352,6 @@
     <t>WWE</t>
   </si>
   <si>
-    <t>CMST</t>
-  </si>
-  <si>
     <t>SFIX</t>
   </si>
   <si>
@@ -692,13 +695,16 @@
   </si>
   <si>
     <t>0001759509</t>
+  </si>
+  <si>
+    <t>CMCSA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -761,6 +767,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -807,7 +821,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -839,9 +853,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -873,6 +905,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1048,14 +1098,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1099,7 +1151,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1140,10 +1192,10 @@
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1184,10 +1236,10 @@
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1228,10 +1280,10 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1272,10 +1324,10 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1316,10 +1368,10 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1360,10 +1412,10 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1404,10 +1456,10 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1448,10 +1500,10 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1492,10 +1544,10 @@
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1536,10 +1588,10 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -1580,10 +1632,10 @@
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1624,10 +1676,10 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -1668,10 +1720,10 @@
         <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1712,10 +1764,10 @@
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1756,10 +1808,10 @@
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -1800,10 +1852,10 @@
         <v>1</v>
       </c>
       <c r="N17" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1844,10 +1896,10 @@
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1888,10 +1940,10 @@
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -1932,10 +1984,10 @@
         <v>1</v>
       </c>
       <c r="N20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -1976,10 +2028,10 @@
         <v>1</v>
       </c>
       <c r="N21" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -2020,10 +2072,10 @@
         <v>1</v>
       </c>
       <c r="N22" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
@@ -2064,10 +2116,10 @@
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -2108,10 +2160,10 @@
         <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
@@ -2152,10 +2204,10 @@
         <v>1</v>
       </c>
       <c r="N25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
@@ -2196,10 +2248,10 @@
         <v>1</v>
       </c>
       <c r="N26" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
@@ -2240,10 +2292,10 @@
         <v>1</v>
       </c>
       <c r="N27" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
@@ -2284,10 +2336,10 @@
         <v>1</v>
       </c>
       <c r="N28" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -2328,10 +2380,10 @@
         <v>1</v>
       </c>
       <c r="N29" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>42</v>
       </c>
@@ -2372,10 +2424,10 @@
         <v>1</v>
       </c>
       <c r="N30" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>43</v>
       </c>
@@ -2416,10 +2468,10 @@
         <v>1</v>
       </c>
       <c r="N31" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -2460,10 +2512,10 @@
         <v>1</v>
       </c>
       <c r="N32" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>45</v>
       </c>
@@ -2504,10 +2556,10 @@
         <v>1</v>
       </c>
       <c r="N33" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -2548,10 +2600,10 @@
         <v>1</v>
       </c>
       <c r="N34" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>47</v>
       </c>
@@ -2592,10 +2644,10 @@
         <v>1</v>
       </c>
       <c r="N35" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>48</v>
       </c>
@@ -2636,10 +2688,10 @@
         <v>1</v>
       </c>
       <c r="N36" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>49</v>
       </c>
@@ -2680,10 +2732,10 @@
         <v>1</v>
       </c>
       <c r="N37" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>50</v>
       </c>
@@ -2724,10 +2776,10 @@
         <v>1</v>
       </c>
       <c r="N38" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>51</v>
       </c>
@@ -2768,10 +2820,10 @@
         <v>1</v>
       </c>
       <c r="N39" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>52</v>
       </c>
@@ -2812,10 +2864,10 @@
         <v>1</v>
       </c>
       <c r="N40" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>53</v>
       </c>
@@ -2856,10 +2908,10 @@
         <v>1</v>
       </c>
       <c r="N41" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>54</v>
       </c>
@@ -2900,10 +2952,10 @@
         <v>1</v>
       </c>
       <c r="N42" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>55</v>
       </c>
@@ -2944,10 +2996,10 @@
         <v>1</v>
       </c>
       <c r="N43" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>56</v>
       </c>
@@ -2988,10 +3040,10 @@
         <v>1</v>
       </c>
       <c r="N44" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>57</v>
       </c>
@@ -3032,10 +3084,10 @@
         <v>1</v>
       </c>
       <c r="N45" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>58</v>
       </c>
@@ -3076,10 +3128,10 @@
         <v>1</v>
       </c>
       <c r="N46" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>59</v>
       </c>
@@ -3120,10 +3172,10 @@
         <v>1</v>
       </c>
       <c r="N47" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>60</v>
       </c>
@@ -3164,10 +3216,10 @@
         <v>1</v>
       </c>
       <c r="N48" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>61</v>
       </c>
@@ -3208,10 +3260,10 @@
         <v>1</v>
       </c>
       <c r="N49" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>62</v>
       </c>
@@ -3252,10 +3304,10 @@
         <v>1</v>
       </c>
       <c r="N50" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>63</v>
       </c>
@@ -3296,10 +3348,10 @@
         <v>1</v>
       </c>
       <c r="N51" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>64</v>
       </c>
@@ -3340,10 +3392,10 @@
         <v>1</v>
       </c>
       <c r="N52" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>65</v>
       </c>
@@ -3384,10 +3436,10 @@
         <v>1</v>
       </c>
       <c r="N53" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>66</v>
       </c>
@@ -3428,10 +3480,10 @@
         <v>1</v>
       </c>
       <c r="N54" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>67</v>
       </c>
@@ -3472,10 +3524,10 @@
         <v>1</v>
       </c>
       <c r="N55" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>68</v>
       </c>
@@ -3516,10 +3568,10 @@
         <v>1</v>
       </c>
       <c r="N56" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>69</v>
       </c>
@@ -3560,10 +3612,10 @@
         <v>1</v>
       </c>
       <c r="N57" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>70</v>
       </c>
@@ -3604,10 +3656,10 @@
         <v>1</v>
       </c>
       <c r="N58" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>71</v>
       </c>
@@ -3648,10 +3700,10 @@
         <v>1</v>
       </c>
       <c r="N59" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>72</v>
       </c>
@@ -3692,10 +3744,10 @@
         <v>1</v>
       </c>
       <c r="N60" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>73</v>
       </c>
@@ -3736,10 +3788,10 @@
         <v>1</v>
       </c>
       <c r="N61" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>74</v>
       </c>
@@ -3780,10 +3832,10 @@
         <v>1</v>
       </c>
       <c r="N62" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>75</v>
       </c>
@@ -3824,10 +3876,10 @@
         <v>1</v>
       </c>
       <c r="N63" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>76</v>
       </c>
@@ -3868,10 +3920,10 @@
         <v>1</v>
       </c>
       <c r="N64" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>77</v>
       </c>
@@ -3912,10 +3964,10 @@
         <v>1</v>
       </c>
       <c r="N65" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>78</v>
       </c>
@@ -3956,10 +4008,10 @@
         <v>1</v>
       </c>
       <c r="N66" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>79</v>
       </c>
@@ -4000,10 +4052,10 @@
         <v>1</v>
       </c>
       <c r="N67" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>80</v>
       </c>
@@ -4044,10 +4096,10 @@
         <v>1</v>
       </c>
       <c r="N68" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>81</v>
       </c>
@@ -4088,10 +4140,10 @@
         <v>1</v>
       </c>
       <c r="N69" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>82</v>
       </c>
@@ -4132,10 +4184,10 @@
         <v>1</v>
       </c>
       <c r="N70" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>83</v>
       </c>
@@ -4176,10 +4228,10 @@
         <v>1</v>
       </c>
       <c r="N71" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>84</v>
       </c>
@@ -4220,10 +4272,10 @@
         <v>1</v>
       </c>
       <c r="N72" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>85</v>
       </c>
@@ -4264,10 +4316,10 @@
         <v>1</v>
       </c>
       <c r="N73" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>86</v>
       </c>
@@ -4308,10 +4360,10 @@
         <v>1</v>
       </c>
       <c r="N74" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>87</v>
       </c>
@@ -4352,10 +4404,10 @@
         <v>1</v>
       </c>
       <c r="N75" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>88</v>
       </c>
@@ -4396,10 +4448,10 @@
         <v>1</v>
       </c>
       <c r="N76" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>89</v>
       </c>
@@ -4440,10 +4492,10 @@
         <v>1</v>
       </c>
       <c r="N77" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>90</v>
       </c>
@@ -4484,10 +4536,10 @@
         <v>1</v>
       </c>
       <c r="N78" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>91</v>
       </c>
@@ -4528,10 +4580,10 @@
         <v>1</v>
       </c>
       <c r="N79" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>92</v>
       </c>
@@ -4572,10 +4624,10 @@
         <v>1</v>
       </c>
       <c r="N80" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>93</v>
       </c>
@@ -4616,10 +4668,10 @@
         <v>1</v>
       </c>
       <c r="N81" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>94</v>
       </c>
@@ -4660,10 +4712,10 @@
         <v>1</v>
       </c>
       <c r="N82" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>95</v>
       </c>
@@ -4704,10 +4756,10 @@
         <v>1</v>
       </c>
       <c r="N83" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>96</v>
       </c>
@@ -4748,10 +4800,10 @@
         <v>1</v>
       </c>
       <c r="N84" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>97</v>
       </c>
@@ -4792,10 +4844,10 @@
         <v>1</v>
       </c>
       <c r="N85" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>98</v>
       </c>
@@ -4836,10 +4888,10 @@
         <v>1</v>
       </c>
       <c r="N86" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>99</v>
       </c>
@@ -4880,10 +4932,10 @@
         <v>1</v>
       </c>
       <c r="N87" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>100</v>
       </c>
@@ -4924,10 +4976,10 @@
         <v>1</v>
       </c>
       <c r="N88" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>101</v>
       </c>
@@ -4968,10 +5020,10 @@
         <v>1</v>
       </c>
       <c r="N89" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>102</v>
       </c>
@@ -5012,10 +5064,10 @@
         <v>1</v>
       </c>
       <c r="N90" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>103</v>
       </c>
@@ -5056,10 +5108,10 @@
         <v>1</v>
       </c>
       <c r="N91" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>104</v>
       </c>
@@ -5100,10 +5152,10 @@
         <v>1</v>
       </c>
       <c r="N92" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>105</v>
       </c>
@@ -5144,10 +5196,10 @@
         <v>1</v>
       </c>
       <c r="N93" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>106</v>
       </c>
@@ -5188,10 +5240,10 @@
         <v>1</v>
       </c>
       <c r="N94" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>107</v>
       </c>
@@ -5232,10 +5284,10 @@
         <v>1</v>
       </c>
       <c r="N95" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>108</v>
       </c>
@@ -5276,10 +5328,10 @@
         <v>1</v>
       </c>
       <c r="N96" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>109</v>
       </c>
@@ -5320,447 +5372,447 @@
         <v>1</v>
       </c>
       <c r="N97" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B98" t="b">
+        <v>1</v>
+      </c>
+      <c r="C98" t="b">
+        <v>1</v>
+      </c>
+      <c r="D98" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" t="b">
+        <v>0</v>
+      </c>
+      <c r="G98" t="b">
+        <v>0</v>
+      </c>
+      <c r="H98" t="b">
+        <v>0</v>
+      </c>
+      <c r="I98" t="b">
+        <v>0</v>
+      </c>
+      <c r="J98" t="b">
+        <v>0</v>
+      </c>
+      <c r="K98" t="b">
+        <v>0</v>
+      </c>
+      <c r="L98" t="b">
+        <v>0</v>
+      </c>
+      <c r="M98" t="b">
+        <v>1</v>
+      </c>
+      <c r="N98" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="98" spans="1:14">
-      <c r="A98" s="1" t="s">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B98" t="b">
-        <v>1</v>
-      </c>
-      <c r="C98" t="b">
-        <v>1</v>
-      </c>
-      <c r="D98" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" t="b">
-        <v>1</v>
-      </c>
-      <c r="F98" t="b">
-        <v>0</v>
-      </c>
-      <c r="G98" t="b">
-        <v>0</v>
-      </c>
-      <c r="H98" t="b">
-        <v>0</v>
-      </c>
-      <c r="I98" t="b">
-        <v>0</v>
-      </c>
-      <c r="J98" t="b">
-        <v>0</v>
-      </c>
-      <c r="K98" t="b">
-        <v>0</v>
-      </c>
-      <c r="L98" t="b">
-        <v>0</v>
-      </c>
-      <c r="M98" t="b">
-        <v>1</v>
-      </c>
-      <c r="N98" t="s">
+      <c r="B99" t="b">
+        <v>0</v>
+      </c>
+      <c r="C99" t="b">
+        <v>0</v>
+      </c>
+      <c r="D99" t="b">
+        <v>0</v>
+      </c>
+      <c r="E99" t="b">
+        <v>0</v>
+      </c>
+      <c r="F99" t="b">
+        <v>0</v>
+      </c>
+      <c r="G99" t="b">
+        <v>0</v>
+      </c>
+      <c r="H99" t="b">
+        <v>0</v>
+      </c>
+      <c r="I99" t="b">
+        <v>0</v>
+      </c>
+      <c r="J99" t="b">
+        <v>0</v>
+      </c>
+      <c r="K99" t="b">
+        <v>0</v>
+      </c>
+      <c r="L99" t="b">
+        <v>0</v>
+      </c>
+      <c r="M99" t="b">
+        <v>0</v>
+      </c>
+      <c r="N99" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="99" spans="1:14">
-      <c r="A99" s="1" t="s">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B99" t="b">
-        <v>0</v>
-      </c>
-      <c r="C99" t="b">
-        <v>0</v>
-      </c>
-      <c r="D99" t="b">
-        <v>0</v>
-      </c>
-      <c r="E99" t="b">
-        <v>0</v>
-      </c>
-      <c r="F99" t="b">
-        <v>0</v>
-      </c>
-      <c r="G99" t="b">
-        <v>0</v>
-      </c>
-      <c r="H99" t="b">
-        <v>0</v>
-      </c>
-      <c r="I99" t="b">
-        <v>0</v>
-      </c>
-      <c r="J99" t="b">
-        <v>0</v>
-      </c>
-      <c r="K99" t="b">
-        <v>0</v>
-      </c>
-      <c r="L99" t="b">
-        <v>0</v>
-      </c>
-      <c r="M99" t="b">
-        <v>0</v>
-      </c>
-      <c r="N99" t="s">
+      <c r="B100" t="b">
+        <v>0</v>
+      </c>
+      <c r="C100" t="b">
+        <v>0</v>
+      </c>
+      <c r="D100" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" t="b">
+        <v>0</v>
+      </c>
+      <c r="F100" t="b">
+        <v>0</v>
+      </c>
+      <c r="G100" t="b">
+        <v>0</v>
+      </c>
+      <c r="H100" t="b">
+        <v>0</v>
+      </c>
+      <c r="I100" t="b">
+        <v>0</v>
+      </c>
+      <c r="J100" t="b">
+        <v>0</v>
+      </c>
+      <c r="K100" t="b">
+        <v>0</v>
+      </c>
+      <c r="L100" t="b">
+        <v>0</v>
+      </c>
+      <c r="M100" t="b">
+        <v>0</v>
+      </c>
+      <c r="N100" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="100" spans="1:14">
-      <c r="A100" s="1" t="s">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B100" t="b">
-        <v>0</v>
-      </c>
-      <c r="C100" t="b">
-        <v>0</v>
-      </c>
-      <c r="D100" t="b">
-        <v>0</v>
-      </c>
-      <c r="E100" t="b">
-        <v>0</v>
-      </c>
-      <c r="F100" t="b">
-        <v>0</v>
-      </c>
-      <c r="G100" t="b">
-        <v>0</v>
-      </c>
-      <c r="H100" t="b">
-        <v>0</v>
-      </c>
-      <c r="I100" t="b">
-        <v>0</v>
-      </c>
-      <c r="J100" t="b">
-        <v>0</v>
-      </c>
-      <c r="K100" t="b">
-        <v>0</v>
-      </c>
-      <c r="L100" t="b">
-        <v>0</v>
-      </c>
-      <c r="M100" t="b">
-        <v>0</v>
-      </c>
-      <c r="N100" t="s">
+      <c r="B101" t="b">
+        <v>0</v>
+      </c>
+      <c r="C101" t="b">
+        <v>0</v>
+      </c>
+      <c r="D101" t="b">
+        <v>0</v>
+      </c>
+      <c r="E101" t="b">
+        <v>0</v>
+      </c>
+      <c r="F101" t="b">
+        <v>0</v>
+      </c>
+      <c r="G101" t="b">
+        <v>0</v>
+      </c>
+      <c r="H101" t="b">
+        <v>0</v>
+      </c>
+      <c r="I101" t="b">
+        <v>0</v>
+      </c>
+      <c r="J101" t="b">
+        <v>0</v>
+      </c>
+      <c r="K101" t="b">
+        <v>0</v>
+      </c>
+      <c r="L101" t="b">
+        <v>0</v>
+      </c>
+      <c r="M101" t="b">
+        <v>0</v>
+      </c>
+      <c r="N101" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="101" spans="1:14">
-      <c r="A101" s="1" t="s">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B101" t="b">
-        <v>0</v>
-      </c>
-      <c r="C101" t="b">
-        <v>0</v>
-      </c>
-      <c r="D101" t="b">
-        <v>0</v>
-      </c>
-      <c r="E101" t="b">
-        <v>0</v>
-      </c>
-      <c r="F101" t="b">
-        <v>0</v>
-      </c>
-      <c r="G101" t="b">
-        <v>0</v>
-      </c>
-      <c r="H101" t="b">
-        <v>0</v>
-      </c>
-      <c r="I101" t="b">
-        <v>0</v>
-      </c>
-      <c r="J101" t="b">
-        <v>0</v>
-      </c>
-      <c r="K101" t="b">
-        <v>0</v>
-      </c>
-      <c r="L101" t="b">
-        <v>0</v>
-      </c>
-      <c r="M101" t="b">
-        <v>0</v>
-      </c>
-      <c r="N101" t="s">
+      <c r="B102" t="b">
+        <v>0</v>
+      </c>
+      <c r="C102" t="b">
+        <v>0</v>
+      </c>
+      <c r="D102" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102" t="b">
+        <v>0</v>
+      </c>
+      <c r="F102" t="b">
+        <v>0</v>
+      </c>
+      <c r="G102" t="b">
+        <v>0</v>
+      </c>
+      <c r="H102" t="b">
+        <v>0</v>
+      </c>
+      <c r="I102" t="b">
+        <v>0</v>
+      </c>
+      <c r="J102" t="b">
+        <v>0</v>
+      </c>
+      <c r="K102" t="b">
+        <v>0</v>
+      </c>
+      <c r="L102" t="b">
+        <v>0</v>
+      </c>
+      <c r="M102" t="b">
+        <v>0</v>
+      </c>
+      <c r="N102" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="102" spans="1:14">
-      <c r="A102" s="1" t="s">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B102" t="b">
-        <v>0</v>
-      </c>
-      <c r="C102" t="b">
-        <v>0</v>
-      </c>
-      <c r="D102" t="b">
-        <v>0</v>
-      </c>
-      <c r="E102" t="b">
-        <v>0</v>
-      </c>
-      <c r="F102" t="b">
-        <v>0</v>
-      </c>
-      <c r="G102" t="b">
-        <v>0</v>
-      </c>
-      <c r="H102" t="b">
-        <v>0</v>
-      </c>
-      <c r="I102" t="b">
-        <v>0</v>
-      </c>
-      <c r="J102" t="b">
-        <v>0</v>
-      </c>
-      <c r="K102" t="b">
-        <v>0</v>
-      </c>
-      <c r="L102" t="b">
-        <v>0</v>
-      </c>
-      <c r="M102" t="b">
-        <v>0</v>
-      </c>
-      <c r="N102" t="s">
+      <c r="B103" t="b">
+        <v>0</v>
+      </c>
+      <c r="C103" t="b">
+        <v>0</v>
+      </c>
+      <c r="D103" t="b">
+        <v>0</v>
+      </c>
+      <c r="E103" t="b">
+        <v>0</v>
+      </c>
+      <c r="F103" t="b">
+        <v>0</v>
+      </c>
+      <c r="G103" t="b">
+        <v>0</v>
+      </c>
+      <c r="H103" t="b">
+        <v>0</v>
+      </c>
+      <c r="I103" t="b">
+        <v>0</v>
+      </c>
+      <c r="J103" t="b">
+        <v>0</v>
+      </c>
+      <c r="K103" t="b">
+        <v>0</v>
+      </c>
+      <c r="L103" t="b">
+        <v>0</v>
+      </c>
+      <c r="M103" t="b">
+        <v>0</v>
+      </c>
+      <c r="N103" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="103" spans="1:14">
-      <c r="A103" s="1" t="s">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B103" t="b">
-        <v>0</v>
-      </c>
-      <c r="C103" t="b">
-        <v>0</v>
-      </c>
-      <c r="D103" t="b">
-        <v>0</v>
-      </c>
-      <c r="E103" t="b">
-        <v>0</v>
-      </c>
-      <c r="F103" t="b">
-        <v>0</v>
-      </c>
-      <c r="G103" t="b">
-        <v>0</v>
-      </c>
-      <c r="H103" t="b">
-        <v>0</v>
-      </c>
-      <c r="I103" t="b">
-        <v>0</v>
-      </c>
-      <c r="J103" t="b">
-        <v>0</v>
-      </c>
-      <c r="K103" t="b">
-        <v>0</v>
-      </c>
-      <c r="L103" t="b">
-        <v>0</v>
-      </c>
-      <c r="M103" t="b">
-        <v>0</v>
-      </c>
-      <c r="N103" t="s">
+      <c r="B104" t="b">
+        <v>0</v>
+      </c>
+      <c r="C104" t="b">
+        <v>0</v>
+      </c>
+      <c r="D104" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104" t="b">
+        <v>0</v>
+      </c>
+      <c r="F104" t="b">
+        <v>0</v>
+      </c>
+      <c r="G104" t="b">
+        <v>0</v>
+      </c>
+      <c r="H104" t="b">
+        <v>0</v>
+      </c>
+      <c r="I104" t="b">
+        <v>0</v>
+      </c>
+      <c r="J104" t="b">
+        <v>0</v>
+      </c>
+      <c r="K104" t="b">
+        <v>0</v>
+      </c>
+      <c r="L104" t="b">
+        <v>0</v>
+      </c>
+      <c r="M104" t="b">
+        <v>0</v>
+      </c>
+      <c r="N104" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="104" spans="1:14">
-      <c r="A104" s="1" t="s">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B104" t="b">
-        <v>0</v>
-      </c>
-      <c r="C104" t="b">
-        <v>0</v>
-      </c>
-      <c r="D104" t="b">
-        <v>0</v>
-      </c>
-      <c r="E104" t="b">
-        <v>0</v>
-      </c>
-      <c r="F104" t="b">
-        <v>0</v>
-      </c>
-      <c r="G104" t="b">
-        <v>0</v>
-      </c>
-      <c r="H104" t="b">
-        <v>0</v>
-      </c>
-      <c r="I104" t="b">
-        <v>0</v>
-      </c>
-      <c r="J104" t="b">
-        <v>0</v>
-      </c>
-      <c r="K104" t="b">
-        <v>0</v>
-      </c>
-      <c r="L104" t="b">
-        <v>0</v>
-      </c>
-      <c r="M104" t="b">
-        <v>0</v>
-      </c>
-      <c r="N104" t="s">
+      <c r="B105" t="b">
+        <v>0</v>
+      </c>
+      <c r="C105" t="b">
+        <v>0</v>
+      </c>
+      <c r="D105" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105" t="b">
+        <v>0</v>
+      </c>
+      <c r="F105" t="b">
+        <v>0</v>
+      </c>
+      <c r="G105" t="b">
+        <v>0</v>
+      </c>
+      <c r="H105" t="b">
+        <v>0</v>
+      </c>
+      <c r="I105" t="b">
+        <v>0</v>
+      </c>
+      <c r="J105" t="b">
+        <v>0</v>
+      </c>
+      <c r="K105" t="b">
+        <v>0</v>
+      </c>
+      <c r="L105" t="b">
+        <v>0</v>
+      </c>
+      <c r="M105" t="b">
+        <v>0</v>
+      </c>
+      <c r="N105" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="105" spans="1:14">
-      <c r="A105" s="1" t="s">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B105" t="b">
-        <v>0</v>
-      </c>
-      <c r="C105" t="b">
-        <v>0</v>
-      </c>
-      <c r="D105" t="b">
-        <v>0</v>
-      </c>
-      <c r="E105" t="b">
-        <v>0</v>
-      </c>
-      <c r="F105" t="b">
-        <v>0</v>
-      </c>
-      <c r="G105" t="b">
-        <v>0</v>
-      </c>
-      <c r="H105" t="b">
-        <v>0</v>
-      </c>
-      <c r="I105" t="b">
-        <v>0</v>
-      </c>
-      <c r="J105" t="b">
-        <v>0</v>
-      </c>
-      <c r="K105" t="b">
-        <v>0</v>
-      </c>
-      <c r="L105" t="b">
-        <v>0</v>
-      </c>
-      <c r="M105" t="b">
-        <v>0</v>
-      </c>
-      <c r="N105" t="s">
+      <c r="B106" t="b">
+        <v>0</v>
+      </c>
+      <c r="C106" t="b">
+        <v>0</v>
+      </c>
+      <c r="D106" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106" t="b">
+        <v>0</v>
+      </c>
+      <c r="F106" t="b">
+        <v>0</v>
+      </c>
+      <c r="G106" t="b">
+        <v>0</v>
+      </c>
+      <c r="H106" t="b">
+        <v>0</v>
+      </c>
+      <c r="I106" t="b">
+        <v>0</v>
+      </c>
+      <c r="J106" t="b">
+        <v>0</v>
+      </c>
+      <c r="K106" t="b">
+        <v>0</v>
+      </c>
+      <c r="L106" t="b">
+        <v>0</v>
+      </c>
+      <c r="M106" t="b">
+        <v>0</v>
+      </c>
+      <c r="N106" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="106" spans="1:14">
-      <c r="A106" s="1" t="s">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B106" t="b">
-        <v>0</v>
-      </c>
-      <c r="C106" t="b">
-        <v>0</v>
-      </c>
-      <c r="D106" t="b">
-        <v>0</v>
-      </c>
-      <c r="E106" t="b">
-        <v>0</v>
-      </c>
-      <c r="F106" t="b">
-        <v>0</v>
-      </c>
-      <c r="G106" t="b">
-        <v>0</v>
-      </c>
-      <c r="H106" t="b">
-        <v>0</v>
-      </c>
-      <c r="I106" t="b">
-        <v>0</v>
-      </c>
-      <c r="J106" t="b">
-        <v>0</v>
-      </c>
-      <c r="K106" t="b">
-        <v>0</v>
-      </c>
-      <c r="L106" t="b">
-        <v>0</v>
-      </c>
-      <c r="M106" t="b">
-        <v>0</v>
-      </c>
-      <c r="N106" t="s">
+      <c r="B107" t="b">
+        <v>0</v>
+      </c>
+      <c r="C107" t="b">
+        <v>0</v>
+      </c>
+      <c r="D107" t="b">
+        <v>0</v>
+      </c>
+      <c r="E107" t="b">
+        <v>0</v>
+      </c>
+      <c r="F107" t="b">
+        <v>0</v>
+      </c>
+      <c r="G107" t="b">
+        <v>0</v>
+      </c>
+      <c r="H107" t="b">
+        <v>0</v>
+      </c>
+      <c r="I107" t="b">
+        <v>0</v>
+      </c>
+      <c r="J107" t="b">
+        <v>0</v>
+      </c>
+      <c r="K107" t="b">
+        <v>0</v>
+      </c>
+      <c r="L107" t="b">
+        <v>0</v>
+      </c>
+      <c r="M107" t="b">
+        <v>0</v>
+      </c>
+      <c r="N107" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="107" spans="1:14">
-      <c r="A107" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B107" t="b">
-        <v>0</v>
-      </c>
-      <c r="C107" t="b">
-        <v>0</v>
-      </c>
-      <c r="D107" t="b">
-        <v>0</v>
-      </c>
-      <c r="E107" t="b">
-        <v>0</v>
-      </c>
-      <c r="F107" t="b">
-        <v>0</v>
-      </c>
-      <c r="G107" t="b">
-        <v>0</v>
-      </c>
-      <c r="H107" t="b">
-        <v>0</v>
-      </c>
-      <c r="I107" t="b">
-        <v>0</v>
-      </c>
-      <c r="J107" t="b">
-        <v>0</v>
-      </c>
-      <c r="K107" t="b">
-        <v>0</v>
-      </c>
-      <c r="L107" t="b">
-        <v>0</v>
-      </c>
-      <c r="M107" t="b">
-        <v>0</v>
-      </c>
-      <c r="N107" t="s">
-        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
End of Day (2)
</commit_message>
<xml_diff>
--- a/Data/Logs/Collected.xlsx
+++ b/Data/Logs/Collected.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/george/Dropbox/Mac/Desktop/Projects/Capstone/Langague-Analysis/Data/Logs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A345FC70-1E89-F345-9B3E-3F2D1F387D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -352,6 +346,9 @@
     <t>WWE</t>
   </si>
   <si>
+    <t>CMCSA</t>
+  </si>
+  <si>
     <t>SFIX</t>
   </si>
   <si>
@@ -695,16 +692,13 @@
   </si>
   <si>
     <t>0001759509</t>
-  </si>
-  <si>
-    <t>CMCSA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -767,14 +761,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -821,7 +807,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -853,27 +839,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -905,24 +873,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1098,16 +1048,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1151,7 +1099,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1192,10 +1140,10 @@
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1212,7 +1160,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -1236,10 +1184,10 @@
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1280,10 +1228,10 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1324,10 +1272,10 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1368,10 +1316,10 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1412,10 +1360,10 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1456,10 +1404,10 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1500,10 +1448,10 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1514,13 +1462,13 @@
         <v>1</v>
       </c>
       <c r="D10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -1544,10 +1492,10 @@
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1588,10 +1536,10 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -1632,10 +1580,10 @@
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1676,10 +1624,10 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -1720,10 +1668,10 @@
         <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1764,10 +1712,10 @@
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1808,10 +1756,10 @@
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -1852,10 +1800,10 @@
         <v>1</v>
       </c>
       <c r="N17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1896,10 +1844,10 @@
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1940,10 +1888,10 @@
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -1984,10 +1932,10 @@
         <v>1</v>
       </c>
       <c r="N20" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -2028,10 +1976,10 @@
         <v>1</v>
       </c>
       <c r="N21" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -2072,10 +2020,10 @@
         <v>1</v>
       </c>
       <c r="N22" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
@@ -2116,10 +2064,10 @@
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -2160,10 +2108,10 @@
         <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
@@ -2204,10 +2152,10 @@
         <v>1</v>
       </c>
       <c r="N25" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
@@ -2248,10 +2196,10 @@
         <v>1</v>
       </c>
       <c r="N26" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
@@ -2292,10 +2240,10 @@
         <v>1</v>
       </c>
       <c r="N27" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
@@ -2336,10 +2284,10 @@
         <v>1</v>
       </c>
       <c r="N28" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -2380,10 +2328,10 @@
         <v>1</v>
       </c>
       <c r="N29" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>42</v>
       </c>
@@ -2424,10 +2372,10 @@
         <v>1</v>
       </c>
       <c r="N30" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>43</v>
       </c>
@@ -2468,10 +2416,10 @@
         <v>1</v>
       </c>
       <c r="N31" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -2512,10 +2460,10 @@
         <v>1</v>
       </c>
       <c r="N32" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
         <v>45</v>
       </c>
@@ -2556,10 +2504,10 @@
         <v>1</v>
       </c>
       <c r="N33" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -2600,10 +2548,10 @@
         <v>1</v>
       </c>
       <c r="N34" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" s="1" t="s">
         <v>47</v>
       </c>
@@ -2644,10 +2592,10 @@
         <v>1</v>
       </c>
       <c r="N35" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" s="1" t="s">
         <v>48</v>
       </c>
@@ -2688,10 +2636,10 @@
         <v>1</v>
       </c>
       <c r="N36" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" s="1" t="s">
         <v>49</v>
       </c>
@@ -2732,10 +2680,10 @@
         <v>1</v>
       </c>
       <c r="N37" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" s="1" t="s">
         <v>50</v>
       </c>
@@ -2776,10 +2724,10 @@
         <v>1</v>
       </c>
       <c r="N38" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" s="1" t="s">
         <v>51</v>
       </c>
@@ -2820,10 +2768,10 @@
         <v>1</v>
       </c>
       <c r="N39" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" s="1" t="s">
         <v>52</v>
       </c>
@@ -2864,10 +2812,10 @@
         <v>1</v>
       </c>
       <c r="N40" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" s="1" t="s">
         <v>53</v>
       </c>
@@ -2908,10 +2856,10 @@
         <v>1</v>
       </c>
       <c r="N41" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" s="1" t="s">
         <v>54</v>
       </c>
@@ -2952,10 +2900,10 @@
         <v>1</v>
       </c>
       <c r="N42" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" s="1" t="s">
         <v>55</v>
       </c>
@@ -2972,7 +2920,7 @@
         <v>1</v>
       </c>
       <c r="F43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" t="b">
         <v>0</v>
@@ -2996,10 +2944,10 @@
         <v>1</v>
       </c>
       <c r="N43" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" s="1" t="s">
         <v>56</v>
       </c>
@@ -3040,10 +2988,10 @@
         <v>1</v>
       </c>
       <c r="N44" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
         <v>57</v>
       </c>
@@ -3084,10 +3032,10 @@
         <v>1</v>
       </c>
       <c r="N45" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
         <v>58</v>
       </c>
@@ -3128,10 +3076,10 @@
         <v>1</v>
       </c>
       <c r="N46" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
         <v>59</v>
       </c>
@@ -3172,10 +3120,10 @@
         <v>1</v>
       </c>
       <c r="N47" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
         <v>60</v>
       </c>
@@ -3216,10 +3164,10 @@
         <v>1</v>
       </c>
       <c r="N48" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" s="1" t="s">
         <v>61</v>
       </c>
@@ -3260,10 +3208,10 @@
         <v>1</v>
       </c>
       <c r="N49" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" s="1" t="s">
         <v>62</v>
       </c>
@@ -3277,25 +3225,25 @@
         <v>1</v>
       </c>
       <c r="E50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L50" t="b">
         <v>0</v>
@@ -3304,10 +3252,10 @@
         <v>1</v>
       </c>
       <c r="N50" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51" s="1" t="s">
         <v>63</v>
       </c>
@@ -3348,10 +3296,10 @@
         <v>1</v>
       </c>
       <c r="N51" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52" s="1" t="s">
         <v>64</v>
       </c>
@@ -3392,10 +3340,10 @@
         <v>1</v>
       </c>
       <c r="N52" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" s="1" t="s">
         <v>65</v>
       </c>
@@ -3436,10 +3384,10 @@
         <v>1</v>
       </c>
       <c r="N53" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="A54" s="1" t="s">
         <v>66</v>
       </c>
@@ -3480,10 +3428,10 @@
         <v>1</v>
       </c>
       <c r="N54" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
       <c r="A55" s="1" t="s">
         <v>67</v>
       </c>
@@ -3524,10 +3472,10 @@
         <v>1</v>
       </c>
       <c r="N55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
       <c r="A56" s="1" t="s">
         <v>68</v>
       </c>
@@ -3568,10 +3516,10 @@
         <v>1</v>
       </c>
       <c r="N56" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
       <c r="A57" s="1" t="s">
         <v>69</v>
       </c>
@@ -3612,42 +3560,42 @@
         <v>1</v>
       </c>
       <c r="N57" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
       <c r="A58" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L58" t="b">
         <v>0</v>
@@ -3656,10 +3604,10 @@
         <v>1</v>
       </c>
       <c r="N58" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
       <c r="A59" s="1" t="s">
         <v>71</v>
       </c>
@@ -3700,10 +3648,10 @@
         <v>1</v>
       </c>
       <c r="N59" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
       <c r="A60" s="1" t="s">
         <v>72</v>
       </c>
@@ -3744,10 +3692,10 @@
         <v>1</v>
       </c>
       <c r="N60" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
       <c r="A61" s="1" t="s">
         <v>73</v>
       </c>
@@ -3788,10 +3736,10 @@
         <v>1</v>
       </c>
       <c r="N61" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
       <c r="A62" s="1" t="s">
         <v>74</v>
       </c>
@@ -3805,22 +3753,22 @@
         <v>1</v>
       </c>
       <c r="E62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K62" t="b">
         <v>0</v>
@@ -3832,10 +3780,10 @@
         <v>1</v>
       </c>
       <c r="N62" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
       <c r="A63" s="1" t="s">
         <v>75</v>
       </c>
@@ -3876,10 +3824,10 @@
         <v>1</v>
       </c>
       <c r="N63" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
       <c r="A64" s="1" t="s">
         <v>76</v>
       </c>
@@ -3920,10 +3868,10 @@
         <v>1</v>
       </c>
       <c r="N64" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
       <c r="A65" s="1" t="s">
         <v>77</v>
       </c>
@@ -3964,10 +3912,10 @@
         <v>1</v>
       </c>
       <c r="N65" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
       <c r="A66" s="1" t="s">
         <v>78</v>
       </c>
@@ -4008,10 +3956,10 @@
         <v>1</v>
       </c>
       <c r="N66" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
       <c r="A67" s="1" t="s">
         <v>79</v>
       </c>
@@ -4052,10 +4000,10 @@
         <v>1</v>
       </c>
       <c r="N67" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
       <c r="A68" s="1" t="s">
         <v>80</v>
       </c>
@@ -4096,10 +4044,10 @@
         <v>1</v>
       </c>
       <c r="N68" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
       <c r="A69" s="1" t="s">
         <v>81</v>
       </c>
@@ -4140,10 +4088,10 @@
         <v>1</v>
       </c>
       <c r="N69" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
       <c r="A70" s="1" t="s">
         <v>82</v>
       </c>
@@ -4184,10 +4132,10 @@
         <v>1</v>
       </c>
       <c r="N70" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14">
       <c r="A71" s="1" t="s">
         <v>83</v>
       </c>
@@ -4228,10 +4176,10 @@
         <v>1</v>
       </c>
       <c r="N71" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14">
       <c r="A72" s="1" t="s">
         <v>84</v>
       </c>
@@ -4245,16 +4193,16 @@
         <v>1</v>
       </c>
       <c r="E72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I72" t="b">
         <v>1</v>
@@ -4272,10 +4220,10 @@
         <v>1</v>
       </c>
       <c r="N72" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14">
       <c r="A73" s="1" t="s">
         <v>85</v>
       </c>
@@ -4316,10 +4264,10 @@
         <v>1</v>
       </c>
       <c r="N73" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14">
       <c r="A74" s="1" t="s">
         <v>86</v>
       </c>
@@ -4360,10 +4308,10 @@
         <v>1</v>
       </c>
       <c r="N74" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14">
       <c r="A75" s="1" t="s">
         <v>87</v>
       </c>
@@ -4404,10 +4352,10 @@
         <v>1</v>
       </c>
       <c r="N75" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14">
       <c r="A76" s="1" t="s">
         <v>88</v>
       </c>
@@ -4448,10 +4396,10 @@
         <v>1</v>
       </c>
       <c r="N76" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14">
       <c r="A77" s="1" t="s">
         <v>89</v>
       </c>
@@ -4492,10 +4440,10 @@
         <v>1</v>
       </c>
       <c r="N77" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14">
       <c r="A78" s="1" t="s">
         <v>90</v>
       </c>
@@ -4536,10 +4484,10 @@
         <v>1</v>
       </c>
       <c r="N78" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14">
       <c r="A79" s="1" t="s">
         <v>91</v>
       </c>
@@ -4580,10 +4528,10 @@
         <v>1</v>
       </c>
       <c r="N79" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14">
       <c r="A80" s="1" t="s">
         <v>92</v>
       </c>
@@ -4624,10 +4572,10 @@
         <v>1</v>
       </c>
       <c r="N80" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14">
       <c r="A81" s="1" t="s">
         <v>93</v>
       </c>
@@ -4668,10 +4616,10 @@
         <v>1</v>
       </c>
       <c r="N81" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14">
       <c r="A82" s="1" t="s">
         <v>94</v>
       </c>
@@ -4712,10 +4660,10 @@
         <v>1</v>
       </c>
       <c r="N82" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14">
       <c r="A83" s="1" t="s">
         <v>95</v>
       </c>
@@ -4726,28 +4674,28 @@
         <v>1</v>
       </c>
       <c r="D83" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F83" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G83" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H83" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I83" t="b">
         <v>0</v>
       </c>
       <c r="J83" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K83" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L83" t="b">
         <v>0</v>
@@ -4756,10 +4704,10 @@
         <v>1</v>
       </c>
       <c r="N83" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14">
       <c r="A84" s="1" t="s">
         <v>96</v>
       </c>
@@ -4800,10 +4748,10 @@
         <v>1</v>
       </c>
       <c r="N84" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14">
       <c r="A85" s="1" t="s">
         <v>97</v>
       </c>
@@ -4844,10 +4792,10 @@
         <v>1</v>
       </c>
       <c r="N85" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14">
       <c r="A86" s="1" t="s">
         <v>98</v>
       </c>
@@ -4888,10 +4836,10 @@
         <v>1</v>
       </c>
       <c r="N86" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14">
       <c r="A87" s="1" t="s">
         <v>99</v>
       </c>
@@ -4932,10 +4880,10 @@
         <v>1</v>
       </c>
       <c r="N87" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14">
       <c r="A88" s="1" t="s">
         <v>100</v>
       </c>
@@ -4976,10 +4924,10 @@
         <v>1</v>
       </c>
       <c r="N88" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14">
       <c r="A89" s="1" t="s">
         <v>101</v>
       </c>
@@ -5020,10 +4968,10 @@
         <v>1</v>
       </c>
       <c r="N89" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14">
       <c r="A90" s="1" t="s">
         <v>102</v>
       </c>
@@ -5061,13 +5009,13 @@
         <v>0</v>
       </c>
       <c r="M90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N90" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14">
       <c r="A91" s="1" t="s">
         <v>103</v>
       </c>
@@ -5108,10 +5056,10 @@
         <v>1</v>
       </c>
       <c r="N91" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14">
       <c r="A92" s="1" t="s">
         <v>104</v>
       </c>
@@ -5152,10 +5100,10 @@
         <v>1</v>
       </c>
       <c r="N92" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14">
       <c r="A93" s="1" t="s">
         <v>105</v>
       </c>
@@ -5196,10 +5144,10 @@
         <v>1</v>
       </c>
       <c r="N93" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14">
       <c r="A94" s="1" t="s">
         <v>106</v>
       </c>
@@ -5240,15 +5188,15 @@
         <v>1</v>
       </c>
       <c r="N94" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14">
       <c r="A95" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B95" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C95" t="b">
         <v>1</v>
@@ -5284,10 +5232,10 @@
         <v>1</v>
       </c>
       <c r="N95" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14">
       <c r="A96" s="1" t="s">
         <v>108</v>
       </c>
@@ -5313,13 +5261,13 @@
         <v>0</v>
       </c>
       <c r="I96" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J96" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K96" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L96" t="b">
         <v>0</v>
@@ -5328,10 +5276,10 @@
         <v>1</v>
       </c>
       <c r="N96" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14">
       <c r="A97" s="1" t="s">
         <v>109</v>
       </c>
@@ -5372,447 +5320,447 @@
         <v>1</v>
       </c>
       <c r="N97" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14">
       <c r="A98" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B98" t="b">
+        <v>1</v>
+      </c>
+      <c r="C98" t="b">
+        <v>1</v>
+      </c>
+      <c r="D98" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" t="b">
+        <v>1</v>
+      </c>
+      <c r="G98" t="b">
+        <v>1</v>
+      </c>
+      <c r="H98" t="b">
+        <v>1</v>
+      </c>
+      <c r="I98" t="b">
+        <v>1</v>
+      </c>
+      <c r="J98" t="b">
+        <v>1</v>
+      </c>
+      <c r="K98" t="b">
+        <v>1</v>
+      </c>
+      <c r="L98" t="b">
+        <v>0</v>
+      </c>
+      <c r="M98" t="b">
+        <v>1</v>
+      </c>
+      <c r="N98" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14">
+      <c r="A99" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B99" t="b">
+        <v>1</v>
+      </c>
+      <c r="C99" t="b">
+        <v>1</v>
+      </c>
+      <c r="D99" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" t="b">
+        <v>0</v>
+      </c>
+      <c r="F99" t="b">
+        <v>0</v>
+      </c>
+      <c r="G99" t="b">
+        <v>0</v>
+      </c>
+      <c r="H99" t="b">
+        <v>0</v>
+      </c>
+      <c r="I99" t="b">
+        <v>0</v>
+      </c>
+      <c r="J99" t="b">
+        <v>0</v>
+      </c>
+      <c r="K99" t="b">
+        <v>0</v>
+      </c>
+      <c r="L99" t="b">
+        <v>0</v>
+      </c>
+      <c r="M99" t="b">
+        <v>1</v>
+      </c>
+      <c r="N99" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14">
+      <c r="A100" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B100" t="b">
+        <v>1</v>
+      </c>
+      <c r="C100" t="b">
+        <v>1</v>
+      </c>
+      <c r="D100" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" t="b">
+        <v>0</v>
+      </c>
+      <c r="F100" t="b">
+        <v>0</v>
+      </c>
+      <c r="G100" t="b">
+        <v>0</v>
+      </c>
+      <c r="H100" t="b">
+        <v>0</v>
+      </c>
+      <c r="I100" t="b">
+        <v>0</v>
+      </c>
+      <c r="J100" t="b">
+        <v>0</v>
+      </c>
+      <c r="K100" t="b">
+        <v>0</v>
+      </c>
+      <c r="L100" t="b">
+        <v>0</v>
+      </c>
+      <c r="M100" t="b">
+        <v>1</v>
+      </c>
+      <c r="N100" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14">
+      <c r="A101" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B101" t="b">
+        <v>1</v>
+      </c>
+      <c r="C101" t="b">
+        <v>1</v>
+      </c>
+      <c r="D101" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" t="b">
+        <v>1</v>
+      </c>
+      <c r="F101" t="b">
+        <v>1</v>
+      </c>
+      <c r="G101" t="b">
+        <v>1</v>
+      </c>
+      <c r="H101" t="b">
+        <v>1</v>
+      </c>
+      <c r="I101" t="b">
+        <v>0</v>
+      </c>
+      <c r="J101" t="b">
+        <v>0</v>
+      </c>
+      <c r="K101" t="b">
+        <v>0</v>
+      </c>
+      <c r="L101" t="b">
+        <v>0</v>
+      </c>
+      <c r="M101" t="b">
+        <v>1</v>
+      </c>
+      <c r="N101" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14">
+      <c r="A102" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B102" t="b">
+        <v>1</v>
+      </c>
+      <c r="C102" t="b">
+        <v>1</v>
+      </c>
+      <c r="D102" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" t="b">
+        <v>1</v>
+      </c>
+      <c r="F102" t="b">
+        <v>1</v>
+      </c>
+      <c r="G102" t="b">
+        <v>1</v>
+      </c>
+      <c r="H102" t="b">
+        <v>0</v>
+      </c>
+      <c r="I102" t="b">
+        <v>0</v>
+      </c>
+      <c r="J102" t="b">
+        <v>0</v>
+      </c>
+      <c r="K102" t="b">
+        <v>0</v>
+      </c>
+      <c r="L102" t="b">
+        <v>0</v>
+      </c>
+      <c r="M102" t="b">
+        <v>1</v>
+      </c>
+      <c r="N102" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14">
+      <c r="A103" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B103" t="b">
+        <v>1</v>
+      </c>
+      <c r="C103" t="b">
+        <v>1</v>
+      </c>
+      <c r="D103" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" t="b">
+        <v>1</v>
+      </c>
+      <c r="F103" t="b">
+        <v>1</v>
+      </c>
+      <c r="G103" t="b">
+        <v>1</v>
+      </c>
+      <c r="H103" t="b">
+        <v>1</v>
+      </c>
+      <c r="I103" t="b">
+        <v>0</v>
+      </c>
+      <c r="J103" t="b">
+        <v>0</v>
+      </c>
+      <c r="K103" t="b">
+        <v>0</v>
+      </c>
+      <c r="L103" t="b">
+        <v>0</v>
+      </c>
+      <c r="M103" t="b">
+        <v>1</v>
+      </c>
+      <c r="N103" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14">
+      <c r="A104" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B104" t="b">
+        <v>1</v>
+      </c>
+      <c r="C104" t="b">
+        <v>0</v>
+      </c>
+      <c r="D104" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104" t="b">
+        <v>0</v>
+      </c>
+      <c r="F104" t="b">
+        <v>0</v>
+      </c>
+      <c r="G104" t="b">
+        <v>0</v>
+      </c>
+      <c r="H104" t="b">
+        <v>0</v>
+      </c>
+      <c r="I104" t="b">
+        <v>0</v>
+      </c>
+      <c r="J104" t="b">
+        <v>0</v>
+      </c>
+      <c r="K104" t="b">
+        <v>0</v>
+      </c>
+      <c r="L104" t="b">
+        <v>0</v>
+      </c>
+      <c r="M104" t="b">
+        <v>1</v>
+      </c>
+      <c r="N104" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14">
+      <c r="A105" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B105" t="b">
+        <v>1</v>
+      </c>
+      <c r="C105" t="b">
+        <v>1</v>
+      </c>
+      <c r="D105" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105" t="b">
+        <v>0</v>
+      </c>
+      <c r="F105" t="b">
+        <v>0</v>
+      </c>
+      <c r="G105" t="b">
+        <v>0</v>
+      </c>
+      <c r="H105" t="b">
+        <v>0</v>
+      </c>
+      <c r="I105" t="b">
+        <v>0</v>
+      </c>
+      <c r="J105" t="b">
+        <v>0</v>
+      </c>
+      <c r="K105" t="b">
+        <v>0</v>
+      </c>
+      <c r="L105" t="b">
+        <v>0</v>
+      </c>
+      <c r="M105" t="b">
+        <v>1</v>
+      </c>
+      <c r="N105" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14">
+      <c r="A106" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B106" t="b">
+        <v>1</v>
+      </c>
+      <c r="C106" t="b">
+        <v>0</v>
+      </c>
+      <c r="D106" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106" t="b">
+        <v>0</v>
+      </c>
+      <c r="F106" t="b">
+        <v>0</v>
+      </c>
+      <c r="G106" t="b">
+        <v>0</v>
+      </c>
+      <c r="H106" t="b">
+        <v>0</v>
+      </c>
+      <c r="I106" t="b">
+        <v>0</v>
+      </c>
+      <c r="J106" t="b">
+        <v>0</v>
+      </c>
+      <c r="K106" t="b">
+        <v>0</v>
+      </c>
+      <c r="L106" t="b">
+        <v>0</v>
+      </c>
+      <c r="M106" t="b">
+        <v>1</v>
+      </c>
+      <c r="N106" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14">
+      <c r="A107" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B107" t="b">
+        <v>1</v>
+      </c>
+      <c r="C107" t="b">
+        <v>1</v>
+      </c>
+      <c r="D107" t="b">
+        <v>0</v>
+      </c>
+      <c r="E107" t="b">
+        <v>0</v>
+      </c>
+      <c r="F107" t="b">
+        <v>0</v>
+      </c>
+      <c r="G107" t="b">
+        <v>0</v>
+      </c>
+      <c r="H107" t="b">
+        <v>0</v>
+      </c>
+      <c r="I107" t="b">
+        <v>0</v>
+      </c>
+      <c r="J107" t="b">
+        <v>0</v>
+      </c>
+      <c r="K107" t="b">
+        <v>0</v>
+      </c>
+      <c r="L107" t="b">
+        <v>0</v>
+      </c>
+      <c r="M107" t="b">
+        <v>1</v>
+      </c>
+      <c r="N107" t="s">
         <v>225</v>
-      </c>
-      <c r="B98" t="b">
-        <v>1</v>
-      </c>
-      <c r="C98" t="b">
-        <v>1</v>
-      </c>
-      <c r="D98" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" t="b">
-        <v>1</v>
-      </c>
-      <c r="F98" t="b">
-        <v>0</v>
-      </c>
-      <c r="G98" t="b">
-        <v>0</v>
-      </c>
-      <c r="H98" t="b">
-        <v>0</v>
-      </c>
-      <c r="I98" t="b">
-        <v>0</v>
-      </c>
-      <c r="J98" t="b">
-        <v>0</v>
-      </c>
-      <c r="K98" t="b">
-        <v>0</v>
-      </c>
-      <c r="L98" t="b">
-        <v>0</v>
-      </c>
-      <c r="M98" t="b">
-        <v>1</v>
-      </c>
-      <c r="N98" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B99" t="b">
-        <v>0</v>
-      </c>
-      <c r="C99" t="b">
-        <v>0</v>
-      </c>
-      <c r="D99" t="b">
-        <v>0</v>
-      </c>
-      <c r="E99" t="b">
-        <v>0</v>
-      </c>
-      <c r="F99" t="b">
-        <v>0</v>
-      </c>
-      <c r="G99" t="b">
-        <v>0</v>
-      </c>
-      <c r="H99" t="b">
-        <v>0</v>
-      </c>
-      <c r="I99" t="b">
-        <v>0</v>
-      </c>
-      <c r="J99" t="b">
-        <v>0</v>
-      </c>
-      <c r="K99" t="b">
-        <v>0</v>
-      </c>
-      <c r="L99" t="b">
-        <v>0</v>
-      </c>
-      <c r="M99" t="b">
-        <v>0</v>
-      </c>
-      <c r="N99" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A100" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B100" t="b">
-        <v>0</v>
-      </c>
-      <c r="C100" t="b">
-        <v>0</v>
-      </c>
-      <c r="D100" t="b">
-        <v>0</v>
-      </c>
-      <c r="E100" t="b">
-        <v>0</v>
-      </c>
-      <c r="F100" t="b">
-        <v>0</v>
-      </c>
-      <c r="G100" t="b">
-        <v>0</v>
-      </c>
-      <c r="H100" t="b">
-        <v>0</v>
-      </c>
-      <c r="I100" t="b">
-        <v>0</v>
-      </c>
-      <c r="J100" t="b">
-        <v>0</v>
-      </c>
-      <c r="K100" t="b">
-        <v>0</v>
-      </c>
-      <c r="L100" t="b">
-        <v>0</v>
-      </c>
-      <c r="M100" t="b">
-        <v>0</v>
-      </c>
-      <c r="N100" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A101" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B101" t="b">
-        <v>0</v>
-      </c>
-      <c r="C101" t="b">
-        <v>0</v>
-      </c>
-      <c r="D101" t="b">
-        <v>0</v>
-      </c>
-      <c r="E101" t="b">
-        <v>0</v>
-      </c>
-      <c r="F101" t="b">
-        <v>0</v>
-      </c>
-      <c r="G101" t="b">
-        <v>0</v>
-      </c>
-      <c r="H101" t="b">
-        <v>0</v>
-      </c>
-      <c r="I101" t="b">
-        <v>0</v>
-      </c>
-      <c r="J101" t="b">
-        <v>0</v>
-      </c>
-      <c r="K101" t="b">
-        <v>0</v>
-      </c>
-      <c r="L101" t="b">
-        <v>0</v>
-      </c>
-      <c r="M101" t="b">
-        <v>0</v>
-      </c>
-      <c r="N101" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B102" t="b">
-        <v>0</v>
-      </c>
-      <c r="C102" t="b">
-        <v>0</v>
-      </c>
-      <c r="D102" t="b">
-        <v>0</v>
-      </c>
-      <c r="E102" t="b">
-        <v>0</v>
-      </c>
-      <c r="F102" t="b">
-        <v>0</v>
-      </c>
-      <c r="G102" t="b">
-        <v>0</v>
-      </c>
-      <c r="H102" t="b">
-        <v>0</v>
-      </c>
-      <c r="I102" t="b">
-        <v>0</v>
-      </c>
-      <c r="J102" t="b">
-        <v>0</v>
-      </c>
-      <c r="K102" t="b">
-        <v>0</v>
-      </c>
-      <c r="L102" t="b">
-        <v>0</v>
-      </c>
-      <c r="M102" t="b">
-        <v>0</v>
-      </c>
-      <c r="N102" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A103" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B103" t="b">
-        <v>0</v>
-      </c>
-      <c r="C103" t="b">
-        <v>0</v>
-      </c>
-      <c r="D103" t="b">
-        <v>0</v>
-      </c>
-      <c r="E103" t="b">
-        <v>0</v>
-      </c>
-      <c r="F103" t="b">
-        <v>0</v>
-      </c>
-      <c r="G103" t="b">
-        <v>0</v>
-      </c>
-      <c r="H103" t="b">
-        <v>0</v>
-      </c>
-      <c r="I103" t="b">
-        <v>0</v>
-      </c>
-      <c r="J103" t="b">
-        <v>0</v>
-      </c>
-      <c r="K103" t="b">
-        <v>0</v>
-      </c>
-      <c r="L103" t="b">
-        <v>0</v>
-      </c>
-      <c r="M103" t="b">
-        <v>0</v>
-      </c>
-      <c r="N103" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A104" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B104" t="b">
-        <v>0</v>
-      </c>
-      <c r="C104" t="b">
-        <v>0</v>
-      </c>
-      <c r="D104" t="b">
-        <v>0</v>
-      </c>
-      <c r="E104" t="b">
-        <v>0</v>
-      </c>
-      <c r="F104" t="b">
-        <v>0</v>
-      </c>
-      <c r="G104" t="b">
-        <v>0</v>
-      </c>
-      <c r="H104" t="b">
-        <v>0</v>
-      </c>
-      <c r="I104" t="b">
-        <v>0</v>
-      </c>
-      <c r="J104" t="b">
-        <v>0</v>
-      </c>
-      <c r="K104" t="b">
-        <v>0</v>
-      </c>
-      <c r="L104" t="b">
-        <v>0</v>
-      </c>
-      <c r="M104" t="b">
-        <v>0</v>
-      </c>
-      <c r="N104" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A105" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B105" t="b">
-        <v>0</v>
-      </c>
-      <c r="C105" t="b">
-        <v>0</v>
-      </c>
-      <c r="D105" t="b">
-        <v>0</v>
-      </c>
-      <c r="E105" t="b">
-        <v>0</v>
-      </c>
-      <c r="F105" t="b">
-        <v>0</v>
-      </c>
-      <c r="G105" t="b">
-        <v>0</v>
-      </c>
-      <c r="H105" t="b">
-        <v>0</v>
-      </c>
-      <c r="I105" t="b">
-        <v>0</v>
-      </c>
-      <c r="J105" t="b">
-        <v>0</v>
-      </c>
-      <c r="K105" t="b">
-        <v>0</v>
-      </c>
-      <c r="L105" t="b">
-        <v>0</v>
-      </c>
-      <c r="M105" t="b">
-        <v>0</v>
-      </c>
-      <c r="N105" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A106" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B106" t="b">
-        <v>0</v>
-      </c>
-      <c r="C106" t="b">
-        <v>0</v>
-      </c>
-      <c r="D106" t="b">
-        <v>0</v>
-      </c>
-      <c r="E106" t="b">
-        <v>0</v>
-      </c>
-      <c r="F106" t="b">
-        <v>0</v>
-      </c>
-      <c r="G106" t="b">
-        <v>0</v>
-      </c>
-      <c r="H106" t="b">
-        <v>0</v>
-      </c>
-      <c r="I106" t="b">
-        <v>0</v>
-      </c>
-      <c r="J106" t="b">
-        <v>0</v>
-      </c>
-      <c r="K106" t="b">
-        <v>0</v>
-      </c>
-      <c r="L106" t="b">
-        <v>0</v>
-      </c>
-      <c r="M106" t="b">
-        <v>0</v>
-      </c>
-      <c r="N106" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A107" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B107" t="b">
-        <v>0</v>
-      </c>
-      <c r="C107" t="b">
-        <v>0</v>
-      </c>
-      <c r="D107" t="b">
-        <v>0</v>
-      </c>
-      <c r="E107" t="b">
-        <v>0</v>
-      </c>
-      <c r="F107" t="b">
-        <v>0</v>
-      </c>
-      <c r="G107" t="b">
-        <v>0</v>
-      </c>
-      <c r="H107" t="b">
-        <v>0</v>
-      </c>
-      <c r="I107" t="b">
-        <v>0</v>
-      </c>
-      <c r="J107" t="b">
-        <v>0</v>
-      </c>
-      <c r="K107" t="b">
-        <v>0</v>
-      </c>
-      <c r="L107" t="b">
-        <v>0</v>
-      </c>
-      <c r="M107" t="b">
-        <v>0</v>
-      </c>
-      <c r="N107" t="s">
-        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EoD & More Extraction
See Attempt 7;
</commit_message>
<xml_diff>
--- a/Data/Logs/Collected.xlsx
+++ b/Data/Logs/Collected.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="316">
   <si>
     <t>2020</t>
   </si>
@@ -322,9 +322,6 @@
     <t>IRBT</t>
   </si>
   <si>
-    <t>PLTR</t>
-  </si>
-  <si>
     <t>ROKU</t>
   </si>
   <si>
@@ -376,6 +373,144 @@
     <t>LYFT</t>
   </si>
   <si>
+    <t>PRPL</t>
+  </si>
+  <si>
+    <t>LOVE</t>
+  </si>
+  <si>
+    <t>KMX</t>
+  </si>
+  <si>
+    <t>ODP</t>
+  </si>
+  <si>
+    <t>NYT</t>
+  </si>
+  <si>
+    <t>RKT</t>
+  </si>
+  <si>
+    <t>WKHS</t>
+  </si>
+  <si>
+    <t>DKNG</t>
+  </si>
+  <si>
+    <t>AMT</t>
+  </si>
+  <si>
+    <t>LUMN</t>
+  </si>
+  <si>
+    <t>FYBR</t>
+  </si>
+  <si>
+    <t>CRSR</t>
+  </si>
+  <si>
+    <t>CCOI</t>
+  </si>
+  <si>
+    <t>CNSL</t>
+  </si>
+  <si>
+    <t>CALX</t>
+  </si>
+  <si>
+    <t>IDT</t>
+  </si>
+  <si>
+    <t>SSTK</t>
+  </si>
+  <si>
+    <t>SSP</t>
+  </si>
+  <si>
+    <t>CMLS</t>
+  </si>
+  <si>
+    <t>NWSA</t>
+  </si>
+  <si>
+    <t>TSQ</t>
+  </si>
+  <si>
+    <t>SGA</t>
+  </si>
+  <si>
+    <t>YELP</t>
+  </si>
+  <si>
+    <t>TWOU</t>
+  </si>
+  <si>
+    <t>SNAP</t>
+  </si>
+  <si>
+    <t>GRPN</t>
+  </si>
+  <si>
+    <t>DBX</t>
+  </si>
+  <si>
+    <t>PCTY</t>
+  </si>
+  <si>
+    <t>BOX</t>
+  </si>
+  <si>
+    <t>CONE</t>
+  </si>
+  <si>
+    <t>COR</t>
+  </si>
+  <si>
+    <t>TREE</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>ENV</t>
+  </si>
+  <si>
+    <t>FISV</t>
+  </si>
+  <si>
+    <t>SGMS</t>
+  </si>
+  <si>
+    <t>TDS</t>
+  </si>
+  <si>
+    <t>USM</t>
+  </si>
+  <si>
+    <t>SHEN</t>
+  </si>
+  <si>
+    <t>MSTR</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>OSTK</t>
+  </si>
+  <si>
+    <t>MELI</t>
+  </si>
+  <si>
+    <t>CVNA</t>
+  </si>
+  <si>
+    <t>MVIS</t>
+  </si>
+  <si>
+    <t>SPSC</t>
+  </si>
+  <si>
     <t>0001580808</t>
   </si>
   <si>
@@ -640,9 +775,6 @@
     <t>0001159167</t>
   </si>
   <si>
-    <t>0001321655</t>
-  </si>
-  <si>
     <t>0001428439</t>
   </si>
   <si>
@@ -692,6 +824,144 @@
   </si>
   <si>
     <t>0001759509</t>
+  </si>
+  <si>
+    <t>0001643953</t>
+  </si>
+  <si>
+    <t>0001701758</t>
+  </si>
+  <si>
+    <t>0001170010</t>
+  </si>
+  <si>
+    <t>0000800240</t>
+  </si>
+  <si>
+    <t>0000071691</t>
+  </si>
+  <si>
+    <t>0001805284</t>
+  </si>
+  <si>
+    <t>0001425287</t>
+  </si>
+  <si>
+    <t>0001772757</t>
+  </si>
+  <si>
+    <t>0001053507</t>
+  </si>
+  <si>
+    <t>0000018926</t>
+  </si>
+  <si>
+    <t>0000020520</t>
+  </si>
+  <si>
+    <t>0001743759</t>
+  </si>
+  <si>
+    <t>0001158324</t>
+  </si>
+  <si>
+    <t>0001304421</t>
+  </si>
+  <si>
+    <t>0001406666</t>
+  </si>
+  <si>
+    <t>0001005731</t>
+  </si>
+  <si>
+    <t>0001549346</t>
+  </si>
+  <si>
+    <t>0000832428</t>
+  </si>
+  <si>
+    <t>0001058623</t>
+  </si>
+  <si>
+    <t>0001564708</t>
+  </si>
+  <si>
+    <t>0001499832</t>
+  </si>
+  <si>
+    <t>0000886136</t>
+  </si>
+  <si>
+    <t>0001345016</t>
+  </si>
+  <si>
+    <t>0001459417</t>
+  </si>
+  <si>
+    <t>0001564408</t>
+  </si>
+  <si>
+    <t>0001490281</t>
+  </si>
+  <si>
+    <t>0001467623</t>
+  </si>
+  <si>
+    <t>0001591698</t>
+  </si>
+  <si>
+    <t>0001372612</t>
+  </si>
+  <si>
+    <t>0001553023</t>
+  </si>
+  <si>
+    <t>0001490892</t>
+  </si>
+  <si>
+    <t>0001434621</t>
+  </si>
+  <si>
+    <t>0001409970</t>
+  </si>
+  <si>
+    <t>0001337619</t>
+  </si>
+  <si>
+    <t>0000798354</t>
+  </si>
+  <si>
+    <t>0000750004</t>
+  </si>
+  <si>
+    <t>0001051512</t>
+  </si>
+  <si>
+    <t>0000821130</t>
+  </si>
+  <si>
+    <t>0000354963</t>
+  </si>
+  <si>
+    <t>0001050446</t>
+  </si>
+  <si>
+    <t>0001616707</t>
+  </si>
+  <si>
+    <t>0001130713</t>
+  </si>
+  <si>
+    <t>0001099590</t>
+  </si>
+  <si>
+    <t>0001690820</t>
+  </si>
+  <si>
+    <t>0000065770</t>
+  </si>
+  <si>
+    <t>0001092699</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1319,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N107"/>
+  <dimension ref="A1:N152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1140,7 +1410,7 @@
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>120</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1184,7 +1454,7 @@
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>121</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1228,7 +1498,7 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>122</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -1272,7 +1542,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -1316,7 +1586,7 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1360,7 +1630,7 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>125</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -1404,7 +1674,7 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>126</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -1448,7 +1718,7 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>127</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -1492,7 +1762,7 @@
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>128</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -1536,7 +1806,7 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1580,7 +1850,7 @@
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>130</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1624,7 +1894,7 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>131</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1668,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>132</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -1712,7 +1982,7 @@
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>133</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1756,7 +2026,7 @@
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>134</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -1800,7 +2070,7 @@
         <v>1</v>
       </c>
       <c r="N17" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1844,7 +2114,7 @@
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>136</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1888,7 +2158,7 @@
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>137</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1932,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="N20" t="s">
-        <v>138</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1976,7 +2246,7 @@
         <v>1</v>
       </c>
       <c r="N21" t="s">
-        <v>139</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -2020,7 +2290,7 @@
         <v>1</v>
       </c>
       <c r="N22" t="s">
-        <v>140</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -2064,7 +2334,7 @@
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>141</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -2108,7 +2378,7 @@
         <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>142</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -2152,7 +2422,7 @@
         <v>1</v>
       </c>
       <c r="N25" t="s">
-        <v>143</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -2196,7 +2466,7 @@
         <v>1</v>
       </c>
       <c r="N26" t="s">
-        <v>144</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -2240,7 +2510,7 @@
         <v>1</v>
       </c>
       <c r="N27" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -2284,7 +2554,7 @@
         <v>1</v>
       </c>
       <c r="N28" t="s">
-        <v>146</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -2328,7 +2598,7 @@
         <v>1</v>
       </c>
       <c r="N29" t="s">
-        <v>147</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -2372,7 +2642,7 @@
         <v>1</v>
       </c>
       <c r="N30" t="s">
-        <v>148</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -2416,7 +2686,7 @@
         <v>1</v>
       </c>
       <c r="N31" t="s">
-        <v>149</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -2460,7 +2730,7 @@
         <v>1</v>
       </c>
       <c r="N32" t="s">
-        <v>150</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -2504,7 +2774,7 @@
         <v>1</v>
       </c>
       <c r="N33" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -2548,7 +2818,7 @@
         <v>1</v>
       </c>
       <c r="N34" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -2592,7 +2862,7 @@
         <v>1</v>
       </c>
       <c r="N35" t="s">
-        <v>153</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -2636,7 +2906,7 @@
         <v>1</v>
       </c>
       <c r="N36" t="s">
-        <v>154</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -2680,7 +2950,7 @@
         <v>1</v>
       </c>
       <c r="N37" t="s">
-        <v>155</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -2724,7 +2994,7 @@
         <v>1</v>
       </c>
       <c r="N38" t="s">
-        <v>156</v>
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -2768,7 +3038,7 @@
         <v>1</v>
       </c>
       <c r="N39" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -2812,7 +3082,7 @@
         <v>1</v>
       </c>
       <c r="N40" t="s">
-        <v>158</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -2856,7 +3126,7 @@
         <v>1</v>
       </c>
       <c r="N41" t="s">
-        <v>159</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -2900,7 +3170,7 @@
         <v>1</v>
       </c>
       <c r="N42" t="s">
-        <v>160</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -2944,7 +3214,7 @@
         <v>1</v>
       </c>
       <c r="N43" t="s">
-        <v>161</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -2988,7 +3258,7 @@
         <v>1</v>
       </c>
       <c r="N44" t="s">
-        <v>162</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -3032,7 +3302,7 @@
         <v>1</v>
       </c>
       <c r="N45" t="s">
-        <v>163</v>
+        <v>208</v>
       </c>
     </row>
     <row r="46" spans="1:14">
@@ -3076,7 +3346,7 @@
         <v>1</v>
       </c>
       <c r="N46" t="s">
-        <v>164</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -3120,7 +3390,7 @@
         <v>1</v>
       </c>
       <c r="N47" t="s">
-        <v>165</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:14">
@@ -3164,7 +3434,7 @@
         <v>1</v>
       </c>
       <c r="N48" t="s">
-        <v>166</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="1:14">
@@ -3208,7 +3478,7 @@
         <v>1</v>
       </c>
       <c r="N49" t="s">
-        <v>167</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="1:14">
@@ -3252,7 +3522,7 @@
         <v>1</v>
       </c>
       <c r="N50" t="s">
-        <v>168</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:14">
@@ -3296,7 +3566,7 @@
         <v>1</v>
       </c>
       <c r="N51" t="s">
-        <v>169</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:14">
@@ -3340,7 +3610,7 @@
         <v>1</v>
       </c>
       <c r="N52" t="s">
-        <v>170</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="1:14">
@@ -3384,7 +3654,7 @@
         <v>1</v>
       </c>
       <c r="N53" t="s">
-        <v>171</v>
+        <v>216</v>
       </c>
     </row>
     <row r="54" spans="1:14">
@@ -3428,7 +3698,7 @@
         <v>1</v>
       </c>
       <c r="N54" t="s">
-        <v>172</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:14">
@@ -3472,7 +3742,7 @@
         <v>1</v>
       </c>
       <c r="N55" t="s">
-        <v>173</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="1:14">
@@ -3516,7 +3786,7 @@
         <v>1</v>
       </c>
       <c r="N56" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
     </row>
     <row r="57" spans="1:14">
@@ -3560,7 +3830,7 @@
         <v>1</v>
       </c>
       <c r="N57" t="s">
-        <v>175</v>
+        <v>220</v>
       </c>
     </row>
     <row r="58" spans="1:14">
@@ -3604,7 +3874,7 @@
         <v>1</v>
       </c>
       <c r="N58" t="s">
-        <v>176</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="1:14">
@@ -3648,7 +3918,7 @@
         <v>1</v>
       </c>
       <c r="N59" t="s">
-        <v>177</v>
+        <v>222</v>
       </c>
     </row>
     <row r="60" spans="1:14">
@@ -3692,7 +3962,7 @@
         <v>1</v>
       </c>
       <c r="N60" t="s">
-        <v>178</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="1:14">
@@ -3736,7 +4006,7 @@
         <v>1</v>
       </c>
       <c r="N61" t="s">
-        <v>179</v>
+        <v>224</v>
       </c>
     </row>
     <row r="62" spans="1:14">
@@ -3780,7 +4050,7 @@
         <v>1</v>
       </c>
       <c r="N62" t="s">
-        <v>180</v>
+        <v>225</v>
       </c>
     </row>
     <row r="63" spans="1:14">
@@ -3824,7 +4094,7 @@
         <v>1</v>
       </c>
       <c r="N63" t="s">
-        <v>181</v>
+        <v>226</v>
       </c>
     </row>
     <row r="64" spans="1:14">
@@ -3868,7 +4138,7 @@
         <v>1</v>
       </c>
       <c r="N64" t="s">
-        <v>182</v>
+        <v>227</v>
       </c>
     </row>
     <row r="65" spans="1:14">
@@ -3912,7 +4182,7 @@
         <v>1</v>
       </c>
       <c r="N65" t="s">
-        <v>183</v>
+        <v>228</v>
       </c>
     </row>
     <row r="66" spans="1:14">
@@ -3956,7 +4226,7 @@
         <v>1</v>
       </c>
       <c r="N66" t="s">
-        <v>184</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="1:14">
@@ -4000,7 +4270,7 @@
         <v>1</v>
       </c>
       <c r="N67" t="s">
-        <v>185</v>
+        <v>230</v>
       </c>
     </row>
     <row r="68" spans="1:14">
@@ -4044,7 +4314,7 @@
         <v>1</v>
       </c>
       <c r="N68" t="s">
-        <v>186</v>
+        <v>231</v>
       </c>
     </row>
     <row r="69" spans="1:14">
@@ -4088,7 +4358,7 @@
         <v>1</v>
       </c>
       <c r="N69" t="s">
-        <v>187</v>
+        <v>232</v>
       </c>
     </row>
     <row r="70" spans="1:14">
@@ -4132,7 +4402,7 @@
         <v>1</v>
       </c>
       <c r="N70" t="s">
-        <v>188</v>
+        <v>233</v>
       </c>
     </row>
     <row r="71" spans="1:14">
@@ -4176,7 +4446,7 @@
         <v>1</v>
       </c>
       <c r="N71" t="s">
-        <v>189</v>
+        <v>234</v>
       </c>
     </row>
     <row r="72" spans="1:14">
@@ -4220,7 +4490,7 @@
         <v>1</v>
       </c>
       <c r="N72" t="s">
-        <v>190</v>
+        <v>235</v>
       </c>
     </row>
     <row r="73" spans="1:14">
@@ -4264,7 +4534,7 @@
         <v>1</v>
       </c>
       <c r="N73" t="s">
-        <v>191</v>
+        <v>236</v>
       </c>
     </row>
     <row r="74" spans="1:14">
@@ -4308,7 +4578,7 @@
         <v>1</v>
       </c>
       <c r="N74" t="s">
-        <v>192</v>
+        <v>237</v>
       </c>
     </row>
     <row r="75" spans="1:14">
@@ -4352,7 +4622,7 @@
         <v>1</v>
       </c>
       <c r="N75" t="s">
-        <v>193</v>
+        <v>238</v>
       </c>
     </row>
     <row r="76" spans="1:14">
@@ -4396,7 +4666,7 @@
         <v>1</v>
       </c>
       <c r="N76" t="s">
-        <v>194</v>
+        <v>239</v>
       </c>
     </row>
     <row r="77" spans="1:14">
@@ -4440,7 +4710,7 @@
         <v>1</v>
       </c>
       <c r="N77" t="s">
-        <v>195</v>
+        <v>240</v>
       </c>
     </row>
     <row r="78" spans="1:14">
@@ -4484,7 +4754,7 @@
         <v>1</v>
       </c>
       <c r="N78" t="s">
-        <v>196</v>
+        <v>241</v>
       </c>
     </row>
     <row r="79" spans="1:14">
@@ -4528,7 +4798,7 @@
         <v>1</v>
       </c>
       <c r="N79" t="s">
-        <v>197</v>
+        <v>242</v>
       </c>
     </row>
     <row r="80" spans="1:14">
@@ -4572,7 +4842,7 @@
         <v>1</v>
       </c>
       <c r="N80" t="s">
-        <v>198</v>
+        <v>243</v>
       </c>
     </row>
     <row r="81" spans="1:14">
@@ -4616,7 +4886,7 @@
         <v>1</v>
       </c>
       <c r="N81" t="s">
-        <v>199</v>
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:14">
@@ -4660,7 +4930,7 @@
         <v>1</v>
       </c>
       <c r="N82" t="s">
-        <v>200</v>
+        <v>245</v>
       </c>
     </row>
     <row r="83" spans="1:14">
@@ -4704,7 +4974,7 @@
         <v>1</v>
       </c>
       <c r="N83" t="s">
-        <v>201</v>
+        <v>246</v>
       </c>
     </row>
     <row r="84" spans="1:14">
@@ -4748,7 +5018,7 @@
         <v>1</v>
       </c>
       <c r="N84" t="s">
-        <v>202</v>
+        <v>247</v>
       </c>
     </row>
     <row r="85" spans="1:14">
@@ -4792,7 +5062,7 @@
         <v>1</v>
       </c>
       <c r="N85" t="s">
-        <v>203</v>
+        <v>248</v>
       </c>
     </row>
     <row r="86" spans="1:14">
@@ -4836,7 +5106,7 @@
         <v>1</v>
       </c>
       <c r="N86" t="s">
-        <v>204</v>
+        <v>249</v>
       </c>
     </row>
     <row r="87" spans="1:14">
@@ -4880,7 +5150,7 @@
         <v>1</v>
       </c>
       <c r="N87" t="s">
-        <v>205</v>
+        <v>250</v>
       </c>
     </row>
     <row r="88" spans="1:14">
@@ -4924,7 +5194,7 @@
         <v>1</v>
       </c>
       <c r="N88" t="s">
-        <v>206</v>
+        <v>251</v>
       </c>
     </row>
     <row r="89" spans="1:14">
@@ -4968,7 +5238,7 @@
         <v>1</v>
       </c>
       <c r="N89" t="s">
-        <v>207</v>
+        <v>252</v>
       </c>
     </row>
     <row r="90" spans="1:14">
@@ -4976,16 +5246,16 @@
         <v>102</v>
       </c>
       <c r="B90" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C90" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D90" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E90" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F90" t="b">
         <v>0</v>
@@ -5009,10 +5279,10 @@
         <v>0</v>
       </c>
       <c r="M90" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N90" t="s">
-        <v>208</v>
+        <v>253</v>
       </c>
     </row>
     <row r="91" spans="1:14">
@@ -5032,22 +5302,22 @@
         <v>1</v>
       </c>
       <c r="F91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L91" t="b">
         <v>0</v>
@@ -5056,7 +5326,7 @@
         <v>1</v>
       </c>
       <c r="N91" t="s">
-        <v>209</v>
+        <v>254</v>
       </c>
     </row>
     <row r="92" spans="1:14">
@@ -5100,7 +5370,7 @@
         <v>1</v>
       </c>
       <c r="N92" t="s">
-        <v>210</v>
+        <v>255</v>
       </c>
     </row>
     <row r="93" spans="1:14">
@@ -5144,7 +5414,7 @@
         <v>1</v>
       </c>
       <c r="N93" t="s">
-        <v>211</v>
+        <v>256</v>
       </c>
     </row>
     <row r="94" spans="1:14">
@@ -5179,7 +5449,7 @@
         <v>1</v>
       </c>
       <c r="K94" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L94" t="b">
         <v>0</v>
@@ -5188,7 +5458,7 @@
         <v>1</v>
       </c>
       <c r="N94" t="s">
-        <v>212</v>
+        <v>257</v>
       </c>
     </row>
     <row r="95" spans="1:14">
@@ -5196,25 +5466,25 @@
         <v>107</v>
       </c>
       <c r="B95" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C95" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D95" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E95" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F95" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G95" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H95" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I95" t="b">
         <v>1</v>
@@ -5223,7 +5493,7 @@
         <v>1</v>
       </c>
       <c r="K95" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L95" t="b">
         <v>0</v>
@@ -5232,7 +5502,7 @@
         <v>1</v>
       </c>
       <c r="N95" t="s">
-        <v>213</v>
+        <v>258</v>
       </c>
     </row>
     <row r="96" spans="1:14">
@@ -5246,19 +5516,19 @@
         <v>0</v>
       </c>
       <c r="D96" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E96" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F96" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G96" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H96" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I96" t="b">
         <v>1</v>
@@ -5267,7 +5537,7 @@
         <v>1</v>
       </c>
       <c r="K96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L96" t="b">
         <v>0</v>
@@ -5276,7 +5546,7 @@
         <v>1</v>
       </c>
       <c r="N96" t="s">
-        <v>214</v>
+        <v>259</v>
       </c>
     </row>
     <row r="97" spans="1:14">
@@ -5284,10 +5554,10 @@
         <v>109</v>
       </c>
       <c r="B97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D97" t="b">
         <v>1</v>
@@ -5311,7 +5581,7 @@
         <v>1</v>
       </c>
       <c r="K97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L97" t="b">
         <v>0</v>
@@ -5320,7 +5590,7 @@
         <v>1</v>
       </c>
       <c r="N97" t="s">
-        <v>215</v>
+        <v>260</v>
       </c>
     </row>
     <row r="98" spans="1:14">
@@ -5337,25 +5607,25 @@
         <v>1</v>
       </c>
       <c r="E98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L98" t="b">
         <v>0</v>
@@ -5364,7 +5634,7 @@
         <v>1</v>
       </c>
       <c r="N98" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
     </row>
     <row r="99" spans="1:14">
@@ -5378,7 +5648,7 @@
         <v>1</v>
       </c>
       <c r="D99" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99" t="b">
         <v>0</v>
@@ -5408,7 +5678,7 @@
         <v>1</v>
       </c>
       <c r="N99" t="s">
-        <v>217</v>
+        <v>262</v>
       </c>
     </row>
     <row r="100" spans="1:14">
@@ -5422,19 +5692,19 @@
         <v>1</v>
       </c>
       <c r="D100" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F100" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G100" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H100" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I100" t="b">
         <v>0</v>
@@ -5452,7 +5722,7 @@
         <v>1</v>
       </c>
       <c r="N100" t="s">
-        <v>218</v>
+        <v>263</v>
       </c>
     </row>
     <row r="101" spans="1:14">
@@ -5478,7 +5748,7 @@
         <v>1</v>
       </c>
       <c r="H101" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I101" t="b">
         <v>0</v>
@@ -5496,7 +5766,7 @@
         <v>1</v>
       </c>
       <c r="N101" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
     </row>
     <row r="102" spans="1:14">
@@ -5522,7 +5792,7 @@
         <v>1</v>
       </c>
       <c r="H102" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I102" t="b">
         <v>0</v>
@@ -5540,7 +5810,7 @@
         <v>1</v>
       </c>
       <c r="N102" t="s">
-        <v>220</v>
+        <v>265</v>
       </c>
     </row>
     <row r="103" spans="1:14">
@@ -5551,22 +5821,22 @@
         <v>1</v>
       </c>
       <c r="C103" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D103" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E103" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F103" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G103" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H103" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I103" t="b">
         <v>0</v>
@@ -5584,7 +5854,7 @@
         <v>1</v>
       </c>
       <c r="N103" t="s">
-        <v>221</v>
+        <v>266</v>
       </c>
     </row>
     <row r="104" spans="1:14">
@@ -5595,7 +5865,7 @@
         <v>1</v>
       </c>
       <c r="C104" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D104" t="b">
         <v>0</v>
@@ -5628,7 +5898,7 @@
         <v>1</v>
       </c>
       <c r="N104" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
     </row>
     <row r="105" spans="1:14">
@@ -5639,7 +5909,7 @@
         <v>1</v>
       </c>
       <c r="C105" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D105" t="b">
         <v>0</v>
@@ -5672,7 +5942,7 @@
         <v>1</v>
       </c>
       <c r="N105" t="s">
-        <v>223</v>
+        <v>268</v>
       </c>
     </row>
     <row r="106" spans="1:14">
@@ -5683,7 +5953,7 @@
         <v>1</v>
       </c>
       <c r="C106" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D106" t="b">
         <v>0</v>
@@ -5716,7 +5986,7 @@
         <v>1</v>
       </c>
       <c r="N106" t="s">
-        <v>224</v>
+        <v>269</v>
       </c>
     </row>
     <row r="107" spans="1:14">
@@ -5724,10 +5994,10 @@
         <v>119</v>
       </c>
       <c r="B107" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C107" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D107" t="b">
         <v>0</v>
@@ -5757,10 +6027,1990 @@
         <v>0</v>
       </c>
       <c r="M107" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N107" t="s">
-        <v>225</v>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14">
+      <c r="A108" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B108" t="b">
+        <v>0</v>
+      </c>
+      <c r="C108" t="b">
+        <v>0</v>
+      </c>
+      <c r="D108" t="b">
+        <v>0</v>
+      </c>
+      <c r="E108" t="b">
+        <v>0</v>
+      </c>
+      <c r="F108" t="b">
+        <v>0</v>
+      </c>
+      <c r="G108" t="b">
+        <v>0</v>
+      </c>
+      <c r="H108" t="b">
+        <v>0</v>
+      </c>
+      <c r="I108" t="b">
+        <v>0</v>
+      </c>
+      <c r="J108" t="b">
+        <v>0</v>
+      </c>
+      <c r="K108" t="b">
+        <v>0</v>
+      </c>
+      <c r="L108" t="b">
+        <v>0</v>
+      </c>
+      <c r="M108" t="b">
+        <v>0</v>
+      </c>
+      <c r="N108" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14">
+      <c r="A109" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B109" t="b">
+        <v>0</v>
+      </c>
+      <c r="C109" t="b">
+        <v>0</v>
+      </c>
+      <c r="D109" t="b">
+        <v>0</v>
+      </c>
+      <c r="E109" t="b">
+        <v>0</v>
+      </c>
+      <c r="F109" t="b">
+        <v>0</v>
+      </c>
+      <c r="G109" t="b">
+        <v>0</v>
+      </c>
+      <c r="H109" t="b">
+        <v>0</v>
+      </c>
+      <c r="I109" t="b">
+        <v>0</v>
+      </c>
+      <c r="J109" t="b">
+        <v>0</v>
+      </c>
+      <c r="K109" t="b">
+        <v>0</v>
+      </c>
+      <c r="L109" t="b">
+        <v>0</v>
+      </c>
+      <c r="M109" t="b">
+        <v>0</v>
+      </c>
+      <c r="N109" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14">
+      <c r="A110" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B110" t="b">
+        <v>0</v>
+      </c>
+      <c r="C110" t="b">
+        <v>0</v>
+      </c>
+      <c r="D110" t="b">
+        <v>0</v>
+      </c>
+      <c r="E110" t="b">
+        <v>0</v>
+      </c>
+      <c r="F110" t="b">
+        <v>0</v>
+      </c>
+      <c r="G110" t="b">
+        <v>0</v>
+      </c>
+      <c r="H110" t="b">
+        <v>0</v>
+      </c>
+      <c r="I110" t="b">
+        <v>0</v>
+      </c>
+      <c r="J110" t="b">
+        <v>0</v>
+      </c>
+      <c r="K110" t="b">
+        <v>0</v>
+      </c>
+      <c r="L110" t="b">
+        <v>0</v>
+      </c>
+      <c r="M110" t="b">
+        <v>0</v>
+      </c>
+      <c r="N110" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14">
+      <c r="A111" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B111" t="b">
+        <v>0</v>
+      </c>
+      <c r="C111" t="b">
+        <v>0</v>
+      </c>
+      <c r="D111" t="b">
+        <v>0</v>
+      </c>
+      <c r="E111" t="b">
+        <v>0</v>
+      </c>
+      <c r="F111" t="b">
+        <v>0</v>
+      </c>
+      <c r="G111" t="b">
+        <v>0</v>
+      </c>
+      <c r="H111" t="b">
+        <v>0</v>
+      </c>
+      <c r="I111" t="b">
+        <v>0</v>
+      </c>
+      <c r="J111" t="b">
+        <v>0</v>
+      </c>
+      <c r="K111" t="b">
+        <v>0</v>
+      </c>
+      <c r="L111" t="b">
+        <v>0</v>
+      </c>
+      <c r="M111" t="b">
+        <v>0</v>
+      </c>
+      <c r="N111" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14">
+      <c r="A112" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B112" t="b">
+        <v>0</v>
+      </c>
+      <c r="C112" t="b">
+        <v>0</v>
+      </c>
+      <c r="D112" t="b">
+        <v>0</v>
+      </c>
+      <c r="E112" t="b">
+        <v>0</v>
+      </c>
+      <c r="F112" t="b">
+        <v>0</v>
+      </c>
+      <c r="G112" t="b">
+        <v>0</v>
+      </c>
+      <c r="H112" t="b">
+        <v>0</v>
+      </c>
+      <c r="I112" t="b">
+        <v>0</v>
+      </c>
+      <c r="J112" t="b">
+        <v>0</v>
+      </c>
+      <c r="K112" t="b">
+        <v>0</v>
+      </c>
+      <c r="L112" t="b">
+        <v>0</v>
+      </c>
+      <c r="M112" t="b">
+        <v>0</v>
+      </c>
+      <c r="N112" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14">
+      <c r="A113" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B113" t="b">
+        <v>0</v>
+      </c>
+      <c r="C113" t="b">
+        <v>0</v>
+      </c>
+      <c r="D113" t="b">
+        <v>0</v>
+      </c>
+      <c r="E113" t="b">
+        <v>0</v>
+      </c>
+      <c r="F113" t="b">
+        <v>0</v>
+      </c>
+      <c r="G113" t="b">
+        <v>0</v>
+      </c>
+      <c r="H113" t="b">
+        <v>0</v>
+      </c>
+      <c r="I113" t="b">
+        <v>0</v>
+      </c>
+      <c r="J113" t="b">
+        <v>0</v>
+      </c>
+      <c r="K113" t="b">
+        <v>0</v>
+      </c>
+      <c r="L113" t="b">
+        <v>0</v>
+      </c>
+      <c r="M113" t="b">
+        <v>0</v>
+      </c>
+      <c r="N113" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14">
+      <c r="A114" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B114" t="b">
+        <v>0</v>
+      </c>
+      <c r="C114" t="b">
+        <v>0</v>
+      </c>
+      <c r="D114" t="b">
+        <v>0</v>
+      </c>
+      <c r="E114" t="b">
+        <v>0</v>
+      </c>
+      <c r="F114" t="b">
+        <v>0</v>
+      </c>
+      <c r="G114" t="b">
+        <v>0</v>
+      </c>
+      <c r="H114" t="b">
+        <v>0</v>
+      </c>
+      <c r="I114" t="b">
+        <v>0</v>
+      </c>
+      <c r="J114" t="b">
+        <v>0</v>
+      </c>
+      <c r="K114" t="b">
+        <v>0</v>
+      </c>
+      <c r="L114" t="b">
+        <v>0</v>
+      </c>
+      <c r="M114" t="b">
+        <v>0</v>
+      </c>
+      <c r="N114" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14">
+      <c r="A115" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B115" t="b">
+        <v>0</v>
+      </c>
+      <c r="C115" t="b">
+        <v>0</v>
+      </c>
+      <c r="D115" t="b">
+        <v>0</v>
+      </c>
+      <c r="E115" t="b">
+        <v>0</v>
+      </c>
+      <c r="F115" t="b">
+        <v>0</v>
+      </c>
+      <c r="G115" t="b">
+        <v>0</v>
+      </c>
+      <c r="H115" t="b">
+        <v>0</v>
+      </c>
+      <c r="I115" t="b">
+        <v>0</v>
+      </c>
+      <c r="J115" t="b">
+        <v>0</v>
+      </c>
+      <c r="K115" t="b">
+        <v>0</v>
+      </c>
+      <c r="L115" t="b">
+        <v>0</v>
+      </c>
+      <c r="M115" t="b">
+        <v>0</v>
+      </c>
+      <c r="N115" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14">
+      <c r="A116" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B116" t="b">
+        <v>0</v>
+      </c>
+      <c r="C116" t="b">
+        <v>0</v>
+      </c>
+      <c r="D116" t="b">
+        <v>0</v>
+      </c>
+      <c r="E116" t="b">
+        <v>0</v>
+      </c>
+      <c r="F116" t="b">
+        <v>0</v>
+      </c>
+      <c r="G116" t="b">
+        <v>0</v>
+      </c>
+      <c r="H116" t="b">
+        <v>0</v>
+      </c>
+      <c r="I116" t="b">
+        <v>0</v>
+      </c>
+      <c r="J116" t="b">
+        <v>0</v>
+      </c>
+      <c r="K116" t="b">
+        <v>0</v>
+      </c>
+      <c r="L116" t="b">
+        <v>0</v>
+      </c>
+      <c r="M116" t="b">
+        <v>0</v>
+      </c>
+      <c r="N116" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14">
+      <c r="A117" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B117" t="b">
+        <v>0</v>
+      </c>
+      <c r="C117" t="b">
+        <v>0</v>
+      </c>
+      <c r="D117" t="b">
+        <v>0</v>
+      </c>
+      <c r="E117" t="b">
+        <v>0</v>
+      </c>
+      <c r="F117" t="b">
+        <v>0</v>
+      </c>
+      <c r="G117" t="b">
+        <v>0</v>
+      </c>
+      <c r="H117" t="b">
+        <v>0</v>
+      </c>
+      <c r="I117" t="b">
+        <v>0</v>
+      </c>
+      <c r="J117" t="b">
+        <v>0</v>
+      </c>
+      <c r="K117" t="b">
+        <v>0</v>
+      </c>
+      <c r="L117" t="b">
+        <v>0</v>
+      </c>
+      <c r="M117" t="b">
+        <v>0</v>
+      </c>
+      <c r="N117" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14">
+      <c r="A118" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B118" t="b">
+        <v>0</v>
+      </c>
+      <c r="C118" t="b">
+        <v>0</v>
+      </c>
+      <c r="D118" t="b">
+        <v>0</v>
+      </c>
+      <c r="E118" t="b">
+        <v>0</v>
+      </c>
+      <c r="F118" t="b">
+        <v>0</v>
+      </c>
+      <c r="G118" t="b">
+        <v>0</v>
+      </c>
+      <c r="H118" t="b">
+        <v>0</v>
+      </c>
+      <c r="I118" t="b">
+        <v>0</v>
+      </c>
+      <c r="J118" t="b">
+        <v>0</v>
+      </c>
+      <c r="K118" t="b">
+        <v>0</v>
+      </c>
+      <c r="L118" t="b">
+        <v>0</v>
+      </c>
+      <c r="M118" t="b">
+        <v>0</v>
+      </c>
+      <c r="N118" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14">
+      <c r="A119" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B119" t="b">
+        <v>0</v>
+      </c>
+      <c r="C119" t="b">
+        <v>0</v>
+      </c>
+      <c r="D119" t="b">
+        <v>0</v>
+      </c>
+      <c r="E119" t="b">
+        <v>0</v>
+      </c>
+      <c r="F119" t="b">
+        <v>0</v>
+      </c>
+      <c r="G119" t="b">
+        <v>0</v>
+      </c>
+      <c r="H119" t="b">
+        <v>0</v>
+      </c>
+      <c r="I119" t="b">
+        <v>0</v>
+      </c>
+      <c r="J119" t="b">
+        <v>0</v>
+      </c>
+      <c r="K119" t="b">
+        <v>0</v>
+      </c>
+      <c r="L119" t="b">
+        <v>0</v>
+      </c>
+      <c r="M119" t="b">
+        <v>0</v>
+      </c>
+      <c r="N119" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14">
+      <c r="A120" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B120" t="b">
+        <v>0</v>
+      </c>
+      <c r="C120" t="b">
+        <v>0</v>
+      </c>
+      <c r="D120" t="b">
+        <v>0</v>
+      </c>
+      <c r="E120" t="b">
+        <v>0</v>
+      </c>
+      <c r="F120" t="b">
+        <v>0</v>
+      </c>
+      <c r="G120" t="b">
+        <v>0</v>
+      </c>
+      <c r="H120" t="b">
+        <v>0</v>
+      </c>
+      <c r="I120" t="b">
+        <v>0</v>
+      </c>
+      <c r="J120" t="b">
+        <v>0</v>
+      </c>
+      <c r="K120" t="b">
+        <v>0</v>
+      </c>
+      <c r="L120" t="b">
+        <v>0</v>
+      </c>
+      <c r="M120" t="b">
+        <v>0</v>
+      </c>
+      <c r="N120" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14">
+      <c r="A121" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B121" t="b">
+        <v>0</v>
+      </c>
+      <c r="C121" t="b">
+        <v>0</v>
+      </c>
+      <c r="D121" t="b">
+        <v>0</v>
+      </c>
+      <c r="E121" t="b">
+        <v>0</v>
+      </c>
+      <c r="F121" t="b">
+        <v>0</v>
+      </c>
+      <c r="G121" t="b">
+        <v>0</v>
+      </c>
+      <c r="H121" t="b">
+        <v>0</v>
+      </c>
+      <c r="I121" t="b">
+        <v>0</v>
+      </c>
+      <c r="J121" t="b">
+        <v>0</v>
+      </c>
+      <c r="K121" t="b">
+        <v>0</v>
+      </c>
+      <c r="L121" t="b">
+        <v>0</v>
+      </c>
+      <c r="M121" t="b">
+        <v>0</v>
+      </c>
+      <c r="N121" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14">
+      <c r="A122" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B122" t="b">
+        <v>0</v>
+      </c>
+      <c r="C122" t="b">
+        <v>0</v>
+      </c>
+      <c r="D122" t="b">
+        <v>0</v>
+      </c>
+      <c r="E122" t="b">
+        <v>0</v>
+      </c>
+      <c r="F122" t="b">
+        <v>0</v>
+      </c>
+      <c r="G122" t="b">
+        <v>0</v>
+      </c>
+      <c r="H122" t="b">
+        <v>0</v>
+      </c>
+      <c r="I122" t="b">
+        <v>0</v>
+      </c>
+      <c r="J122" t="b">
+        <v>0</v>
+      </c>
+      <c r="K122" t="b">
+        <v>0</v>
+      </c>
+      <c r="L122" t="b">
+        <v>0</v>
+      </c>
+      <c r="M122" t="b">
+        <v>0</v>
+      </c>
+      <c r="N122" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14">
+      <c r="A123" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B123" t="b">
+        <v>0</v>
+      </c>
+      <c r="C123" t="b">
+        <v>0</v>
+      </c>
+      <c r="D123" t="b">
+        <v>0</v>
+      </c>
+      <c r="E123" t="b">
+        <v>0</v>
+      </c>
+      <c r="F123" t="b">
+        <v>0</v>
+      </c>
+      <c r="G123" t="b">
+        <v>0</v>
+      </c>
+      <c r="H123" t="b">
+        <v>0</v>
+      </c>
+      <c r="I123" t="b">
+        <v>0</v>
+      </c>
+      <c r="J123" t="b">
+        <v>0</v>
+      </c>
+      <c r="K123" t="b">
+        <v>0</v>
+      </c>
+      <c r="L123" t="b">
+        <v>0</v>
+      </c>
+      <c r="M123" t="b">
+        <v>0</v>
+      </c>
+      <c r="N123" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14">
+      <c r="A124" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B124" t="b">
+        <v>0</v>
+      </c>
+      <c r="C124" t="b">
+        <v>0</v>
+      </c>
+      <c r="D124" t="b">
+        <v>0</v>
+      </c>
+      <c r="E124" t="b">
+        <v>0</v>
+      </c>
+      <c r="F124" t="b">
+        <v>0</v>
+      </c>
+      <c r="G124" t="b">
+        <v>0</v>
+      </c>
+      <c r="H124" t="b">
+        <v>0</v>
+      </c>
+      <c r="I124" t="b">
+        <v>0</v>
+      </c>
+      <c r="J124" t="b">
+        <v>0</v>
+      </c>
+      <c r="K124" t="b">
+        <v>0</v>
+      </c>
+      <c r="L124" t="b">
+        <v>0</v>
+      </c>
+      <c r="M124" t="b">
+        <v>0</v>
+      </c>
+      <c r="N124" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14">
+      <c r="A125" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B125" t="b">
+        <v>0</v>
+      </c>
+      <c r="C125" t="b">
+        <v>0</v>
+      </c>
+      <c r="D125" t="b">
+        <v>0</v>
+      </c>
+      <c r="E125" t="b">
+        <v>0</v>
+      </c>
+      <c r="F125" t="b">
+        <v>0</v>
+      </c>
+      <c r="G125" t="b">
+        <v>0</v>
+      </c>
+      <c r="H125" t="b">
+        <v>0</v>
+      </c>
+      <c r="I125" t="b">
+        <v>0</v>
+      </c>
+      <c r="J125" t="b">
+        <v>0</v>
+      </c>
+      <c r="K125" t="b">
+        <v>0</v>
+      </c>
+      <c r="L125" t="b">
+        <v>0</v>
+      </c>
+      <c r="M125" t="b">
+        <v>0</v>
+      </c>
+      <c r="N125" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14">
+      <c r="A126" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B126" t="b">
+        <v>0</v>
+      </c>
+      <c r="C126" t="b">
+        <v>0</v>
+      </c>
+      <c r="D126" t="b">
+        <v>0</v>
+      </c>
+      <c r="E126" t="b">
+        <v>0</v>
+      </c>
+      <c r="F126" t="b">
+        <v>0</v>
+      </c>
+      <c r="G126" t="b">
+        <v>0</v>
+      </c>
+      <c r="H126" t="b">
+        <v>0</v>
+      </c>
+      <c r="I126" t="b">
+        <v>0</v>
+      </c>
+      <c r="J126" t="b">
+        <v>0</v>
+      </c>
+      <c r="K126" t="b">
+        <v>0</v>
+      </c>
+      <c r="L126" t="b">
+        <v>0</v>
+      </c>
+      <c r="M126" t="b">
+        <v>0</v>
+      </c>
+      <c r="N126" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14">
+      <c r="A127" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B127" t="b">
+        <v>0</v>
+      </c>
+      <c r="C127" t="b">
+        <v>0</v>
+      </c>
+      <c r="D127" t="b">
+        <v>0</v>
+      </c>
+      <c r="E127" t="b">
+        <v>0</v>
+      </c>
+      <c r="F127" t="b">
+        <v>0</v>
+      </c>
+      <c r="G127" t="b">
+        <v>0</v>
+      </c>
+      <c r="H127" t="b">
+        <v>0</v>
+      </c>
+      <c r="I127" t="b">
+        <v>0</v>
+      </c>
+      <c r="J127" t="b">
+        <v>0</v>
+      </c>
+      <c r="K127" t="b">
+        <v>0</v>
+      </c>
+      <c r="L127" t="b">
+        <v>0</v>
+      </c>
+      <c r="M127" t="b">
+        <v>0</v>
+      </c>
+      <c r="N127" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14">
+      <c r="A128" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B128" t="b">
+        <v>0</v>
+      </c>
+      <c r="C128" t="b">
+        <v>0</v>
+      </c>
+      <c r="D128" t="b">
+        <v>0</v>
+      </c>
+      <c r="E128" t="b">
+        <v>0</v>
+      </c>
+      <c r="F128" t="b">
+        <v>0</v>
+      </c>
+      <c r="G128" t="b">
+        <v>0</v>
+      </c>
+      <c r="H128" t="b">
+        <v>0</v>
+      </c>
+      <c r="I128" t="b">
+        <v>0</v>
+      </c>
+      <c r="J128" t="b">
+        <v>0</v>
+      </c>
+      <c r="K128" t="b">
+        <v>0</v>
+      </c>
+      <c r="L128" t="b">
+        <v>0</v>
+      </c>
+      <c r="M128" t="b">
+        <v>0</v>
+      </c>
+      <c r="N128" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14">
+      <c r="A129" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B129" t="b">
+        <v>0</v>
+      </c>
+      <c r="C129" t="b">
+        <v>0</v>
+      </c>
+      <c r="D129" t="b">
+        <v>0</v>
+      </c>
+      <c r="E129" t="b">
+        <v>0</v>
+      </c>
+      <c r="F129" t="b">
+        <v>0</v>
+      </c>
+      <c r="G129" t="b">
+        <v>0</v>
+      </c>
+      <c r="H129" t="b">
+        <v>0</v>
+      </c>
+      <c r="I129" t="b">
+        <v>0</v>
+      </c>
+      <c r="J129" t="b">
+        <v>0</v>
+      </c>
+      <c r="K129" t="b">
+        <v>0</v>
+      </c>
+      <c r="L129" t="b">
+        <v>0</v>
+      </c>
+      <c r="M129" t="b">
+        <v>0</v>
+      </c>
+      <c r="N129" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14">
+      <c r="A130" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B130" t="b">
+        <v>0</v>
+      </c>
+      <c r="C130" t="b">
+        <v>0</v>
+      </c>
+      <c r="D130" t="b">
+        <v>0</v>
+      </c>
+      <c r="E130" t="b">
+        <v>0</v>
+      </c>
+      <c r="F130" t="b">
+        <v>0</v>
+      </c>
+      <c r="G130" t="b">
+        <v>0</v>
+      </c>
+      <c r="H130" t="b">
+        <v>0</v>
+      </c>
+      <c r="I130" t="b">
+        <v>0</v>
+      </c>
+      <c r="J130" t="b">
+        <v>0</v>
+      </c>
+      <c r="K130" t="b">
+        <v>0</v>
+      </c>
+      <c r="L130" t="b">
+        <v>0</v>
+      </c>
+      <c r="M130" t="b">
+        <v>0</v>
+      </c>
+      <c r="N130" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14">
+      <c r="A131" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B131" t="b">
+        <v>0</v>
+      </c>
+      <c r="C131" t="b">
+        <v>0</v>
+      </c>
+      <c r="D131" t="b">
+        <v>0</v>
+      </c>
+      <c r="E131" t="b">
+        <v>0</v>
+      </c>
+      <c r="F131" t="b">
+        <v>0</v>
+      </c>
+      <c r="G131" t="b">
+        <v>0</v>
+      </c>
+      <c r="H131" t="b">
+        <v>0</v>
+      </c>
+      <c r="I131" t="b">
+        <v>0</v>
+      </c>
+      <c r="J131" t="b">
+        <v>0</v>
+      </c>
+      <c r="K131" t="b">
+        <v>0</v>
+      </c>
+      <c r="L131" t="b">
+        <v>0</v>
+      </c>
+      <c r="M131" t="b">
+        <v>0</v>
+      </c>
+      <c r="N131" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14">
+      <c r="A132" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B132" t="b">
+        <v>0</v>
+      </c>
+      <c r="C132" t="b">
+        <v>0</v>
+      </c>
+      <c r="D132" t="b">
+        <v>0</v>
+      </c>
+      <c r="E132" t="b">
+        <v>0</v>
+      </c>
+      <c r="F132" t="b">
+        <v>0</v>
+      </c>
+      <c r="G132" t="b">
+        <v>0</v>
+      </c>
+      <c r="H132" t="b">
+        <v>0</v>
+      </c>
+      <c r="I132" t="b">
+        <v>0</v>
+      </c>
+      <c r="J132" t="b">
+        <v>0</v>
+      </c>
+      <c r="K132" t="b">
+        <v>0</v>
+      </c>
+      <c r="L132" t="b">
+        <v>0</v>
+      </c>
+      <c r="M132" t="b">
+        <v>0</v>
+      </c>
+      <c r="N132" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14">
+      <c r="A133" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B133" t="b">
+        <v>0</v>
+      </c>
+      <c r="C133" t="b">
+        <v>0</v>
+      </c>
+      <c r="D133" t="b">
+        <v>0</v>
+      </c>
+      <c r="E133" t="b">
+        <v>0</v>
+      </c>
+      <c r="F133" t="b">
+        <v>0</v>
+      </c>
+      <c r="G133" t="b">
+        <v>0</v>
+      </c>
+      <c r="H133" t="b">
+        <v>0</v>
+      </c>
+      <c r="I133" t="b">
+        <v>0</v>
+      </c>
+      <c r="J133" t="b">
+        <v>0</v>
+      </c>
+      <c r="K133" t="b">
+        <v>0</v>
+      </c>
+      <c r="L133" t="b">
+        <v>0</v>
+      </c>
+      <c r="M133" t="b">
+        <v>0</v>
+      </c>
+      <c r="N133" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14">
+      <c r="A134" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B134" t="b">
+        <v>0</v>
+      </c>
+      <c r="C134" t="b">
+        <v>0</v>
+      </c>
+      <c r="D134" t="b">
+        <v>0</v>
+      </c>
+      <c r="E134" t="b">
+        <v>0</v>
+      </c>
+      <c r="F134" t="b">
+        <v>0</v>
+      </c>
+      <c r="G134" t="b">
+        <v>0</v>
+      </c>
+      <c r="H134" t="b">
+        <v>0</v>
+      </c>
+      <c r="I134" t="b">
+        <v>0</v>
+      </c>
+      <c r="J134" t="b">
+        <v>0</v>
+      </c>
+      <c r="K134" t="b">
+        <v>0</v>
+      </c>
+      <c r="L134" t="b">
+        <v>0</v>
+      </c>
+      <c r="M134" t="b">
+        <v>0</v>
+      </c>
+      <c r="N134" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14">
+      <c r="A135" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B135" t="b">
+        <v>0</v>
+      </c>
+      <c r="C135" t="b">
+        <v>0</v>
+      </c>
+      <c r="D135" t="b">
+        <v>0</v>
+      </c>
+      <c r="E135" t="b">
+        <v>0</v>
+      </c>
+      <c r="F135" t="b">
+        <v>0</v>
+      </c>
+      <c r="G135" t="b">
+        <v>0</v>
+      </c>
+      <c r="H135" t="b">
+        <v>0</v>
+      </c>
+      <c r="I135" t="b">
+        <v>0</v>
+      </c>
+      <c r="J135" t="b">
+        <v>0</v>
+      </c>
+      <c r="K135" t="b">
+        <v>0</v>
+      </c>
+      <c r="L135" t="b">
+        <v>0</v>
+      </c>
+      <c r="M135" t="b">
+        <v>0</v>
+      </c>
+      <c r="N135" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14">
+      <c r="A136" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B136" t="b">
+        <v>0</v>
+      </c>
+      <c r="C136" t="b">
+        <v>0</v>
+      </c>
+      <c r="D136" t="b">
+        <v>0</v>
+      </c>
+      <c r="E136" t="b">
+        <v>0</v>
+      </c>
+      <c r="F136" t="b">
+        <v>0</v>
+      </c>
+      <c r="G136" t="b">
+        <v>0</v>
+      </c>
+      <c r="H136" t="b">
+        <v>0</v>
+      </c>
+      <c r="I136" t="b">
+        <v>0</v>
+      </c>
+      <c r="J136" t="b">
+        <v>0</v>
+      </c>
+      <c r="K136" t="b">
+        <v>0</v>
+      </c>
+      <c r="L136" t="b">
+        <v>0</v>
+      </c>
+      <c r="M136" t="b">
+        <v>0</v>
+      </c>
+      <c r="N136" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14">
+      <c r="A137" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B137" t="b">
+        <v>0</v>
+      </c>
+      <c r="C137" t="b">
+        <v>0</v>
+      </c>
+      <c r="D137" t="b">
+        <v>0</v>
+      </c>
+      <c r="E137" t="b">
+        <v>0</v>
+      </c>
+      <c r="F137" t="b">
+        <v>0</v>
+      </c>
+      <c r="G137" t="b">
+        <v>0</v>
+      </c>
+      <c r="H137" t="b">
+        <v>0</v>
+      </c>
+      <c r="I137" t="b">
+        <v>0</v>
+      </c>
+      <c r="J137" t="b">
+        <v>0</v>
+      </c>
+      <c r="K137" t="b">
+        <v>0</v>
+      </c>
+      <c r="L137" t="b">
+        <v>0</v>
+      </c>
+      <c r="M137" t="b">
+        <v>0</v>
+      </c>
+      <c r="N137" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14">
+      <c r="A138" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B138" t="b">
+        <v>0</v>
+      </c>
+      <c r="C138" t="b">
+        <v>0</v>
+      </c>
+      <c r="D138" t="b">
+        <v>0</v>
+      </c>
+      <c r="E138" t="b">
+        <v>0</v>
+      </c>
+      <c r="F138" t="b">
+        <v>0</v>
+      </c>
+      <c r="G138" t="b">
+        <v>0</v>
+      </c>
+      <c r="H138" t="b">
+        <v>0</v>
+      </c>
+      <c r="I138" t="b">
+        <v>0</v>
+      </c>
+      <c r="J138" t="b">
+        <v>0</v>
+      </c>
+      <c r="K138" t="b">
+        <v>0</v>
+      </c>
+      <c r="L138" t="b">
+        <v>0</v>
+      </c>
+      <c r="M138" t="b">
+        <v>0</v>
+      </c>
+      <c r="N138" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14">
+      <c r="A139" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B139" t="b">
+        <v>0</v>
+      </c>
+      <c r="C139" t="b">
+        <v>0</v>
+      </c>
+      <c r="D139" t="b">
+        <v>0</v>
+      </c>
+      <c r="E139" t="b">
+        <v>0</v>
+      </c>
+      <c r="F139" t="b">
+        <v>0</v>
+      </c>
+      <c r="G139" t="b">
+        <v>0</v>
+      </c>
+      <c r="H139" t="b">
+        <v>0</v>
+      </c>
+      <c r="I139" t="b">
+        <v>0</v>
+      </c>
+      <c r="J139" t="b">
+        <v>0</v>
+      </c>
+      <c r="K139" t="b">
+        <v>0</v>
+      </c>
+      <c r="L139" t="b">
+        <v>0</v>
+      </c>
+      <c r="M139" t="b">
+        <v>0</v>
+      </c>
+      <c r="N139" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14">
+      <c r="A140" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B140" t="b">
+        <v>0</v>
+      </c>
+      <c r="C140" t="b">
+        <v>0</v>
+      </c>
+      <c r="D140" t="b">
+        <v>0</v>
+      </c>
+      <c r="E140" t="b">
+        <v>0</v>
+      </c>
+      <c r="F140" t="b">
+        <v>0</v>
+      </c>
+      <c r="G140" t="b">
+        <v>0</v>
+      </c>
+      <c r="H140" t="b">
+        <v>0</v>
+      </c>
+      <c r="I140" t="b">
+        <v>0</v>
+      </c>
+      <c r="J140" t="b">
+        <v>0</v>
+      </c>
+      <c r="K140" t="b">
+        <v>0</v>
+      </c>
+      <c r="L140" t="b">
+        <v>0</v>
+      </c>
+      <c r="M140" t="b">
+        <v>0</v>
+      </c>
+      <c r="N140" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14">
+      <c r="A141" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B141" t="b">
+        <v>0</v>
+      </c>
+      <c r="C141" t="b">
+        <v>0</v>
+      </c>
+      <c r="D141" t="b">
+        <v>0</v>
+      </c>
+      <c r="E141" t="b">
+        <v>0</v>
+      </c>
+      <c r="F141" t="b">
+        <v>0</v>
+      </c>
+      <c r="G141" t="b">
+        <v>0</v>
+      </c>
+      <c r="H141" t="b">
+        <v>0</v>
+      </c>
+      <c r="I141" t="b">
+        <v>0</v>
+      </c>
+      <c r="J141" t="b">
+        <v>0</v>
+      </c>
+      <c r="K141" t="b">
+        <v>0</v>
+      </c>
+      <c r="L141" t="b">
+        <v>0</v>
+      </c>
+      <c r="M141" t="b">
+        <v>0</v>
+      </c>
+      <c r="N141" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14">
+      <c r="A142" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B142" t="b">
+        <v>0</v>
+      </c>
+      <c r="C142" t="b">
+        <v>0</v>
+      </c>
+      <c r="D142" t="b">
+        <v>0</v>
+      </c>
+      <c r="E142" t="b">
+        <v>0</v>
+      </c>
+      <c r="F142" t="b">
+        <v>0</v>
+      </c>
+      <c r="G142" t="b">
+        <v>0</v>
+      </c>
+      <c r="H142" t="b">
+        <v>0</v>
+      </c>
+      <c r="I142" t="b">
+        <v>0</v>
+      </c>
+      <c r="J142" t="b">
+        <v>0</v>
+      </c>
+      <c r="K142" t="b">
+        <v>0</v>
+      </c>
+      <c r="L142" t="b">
+        <v>0</v>
+      </c>
+      <c r="M142" t="b">
+        <v>0</v>
+      </c>
+      <c r="N142" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14">
+      <c r="A143" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B143" t="b">
+        <v>0</v>
+      </c>
+      <c r="C143" t="b">
+        <v>0</v>
+      </c>
+      <c r="D143" t="b">
+        <v>0</v>
+      </c>
+      <c r="E143" t="b">
+        <v>0</v>
+      </c>
+      <c r="F143" t="b">
+        <v>0</v>
+      </c>
+      <c r="G143" t="b">
+        <v>0</v>
+      </c>
+      <c r="H143" t="b">
+        <v>0</v>
+      </c>
+      <c r="I143" t="b">
+        <v>0</v>
+      </c>
+      <c r="J143" t="b">
+        <v>0</v>
+      </c>
+      <c r="K143" t="b">
+        <v>0</v>
+      </c>
+      <c r="L143" t="b">
+        <v>0</v>
+      </c>
+      <c r="M143" t="b">
+        <v>0</v>
+      </c>
+      <c r="N143" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14">
+      <c r="A144" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B144" t="b">
+        <v>0</v>
+      </c>
+      <c r="C144" t="b">
+        <v>0</v>
+      </c>
+      <c r="D144" t="b">
+        <v>0</v>
+      </c>
+      <c r="E144" t="b">
+        <v>0</v>
+      </c>
+      <c r="F144" t="b">
+        <v>0</v>
+      </c>
+      <c r="G144" t="b">
+        <v>0</v>
+      </c>
+      <c r="H144" t="b">
+        <v>0</v>
+      </c>
+      <c r="I144" t="b">
+        <v>0</v>
+      </c>
+      <c r="J144" t="b">
+        <v>0</v>
+      </c>
+      <c r="K144" t="b">
+        <v>0</v>
+      </c>
+      <c r="L144" t="b">
+        <v>0</v>
+      </c>
+      <c r="M144" t="b">
+        <v>0</v>
+      </c>
+      <c r="N144" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14">
+      <c r="A145" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B145" t="b">
+        <v>0</v>
+      </c>
+      <c r="C145" t="b">
+        <v>0</v>
+      </c>
+      <c r="D145" t="b">
+        <v>0</v>
+      </c>
+      <c r="E145" t="b">
+        <v>0</v>
+      </c>
+      <c r="F145" t="b">
+        <v>0</v>
+      </c>
+      <c r="G145" t="b">
+        <v>0</v>
+      </c>
+      <c r="H145" t="b">
+        <v>0</v>
+      </c>
+      <c r="I145" t="b">
+        <v>0</v>
+      </c>
+      <c r="J145" t="b">
+        <v>0</v>
+      </c>
+      <c r="K145" t="b">
+        <v>0</v>
+      </c>
+      <c r="L145" t="b">
+        <v>0</v>
+      </c>
+      <c r="M145" t="b">
+        <v>0</v>
+      </c>
+      <c r="N145" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14">
+      <c r="A146" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B146" t="b">
+        <v>0</v>
+      </c>
+      <c r="C146" t="b">
+        <v>0</v>
+      </c>
+      <c r="D146" t="b">
+        <v>0</v>
+      </c>
+      <c r="E146" t="b">
+        <v>0</v>
+      </c>
+      <c r="F146" t="b">
+        <v>0</v>
+      </c>
+      <c r="G146" t="b">
+        <v>0</v>
+      </c>
+      <c r="H146" t="b">
+        <v>0</v>
+      </c>
+      <c r="I146" t="b">
+        <v>0</v>
+      </c>
+      <c r="J146" t="b">
+        <v>0</v>
+      </c>
+      <c r="K146" t="b">
+        <v>0</v>
+      </c>
+      <c r="L146" t="b">
+        <v>0</v>
+      </c>
+      <c r="M146" t="b">
+        <v>0</v>
+      </c>
+      <c r="N146" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14">
+      <c r="A147" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B147" t="b">
+        <v>0</v>
+      </c>
+      <c r="C147" t="b">
+        <v>0</v>
+      </c>
+      <c r="D147" t="b">
+        <v>0</v>
+      </c>
+      <c r="E147" t="b">
+        <v>0</v>
+      </c>
+      <c r="F147" t="b">
+        <v>0</v>
+      </c>
+      <c r="G147" t="b">
+        <v>0</v>
+      </c>
+      <c r="H147" t="b">
+        <v>0</v>
+      </c>
+      <c r="I147" t="b">
+        <v>0</v>
+      </c>
+      <c r="J147" t="b">
+        <v>0</v>
+      </c>
+      <c r="K147" t="b">
+        <v>0</v>
+      </c>
+      <c r="L147" t="b">
+        <v>0</v>
+      </c>
+      <c r="M147" t="b">
+        <v>0</v>
+      </c>
+      <c r="N147" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14">
+      <c r="A148" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B148" t="b">
+        <v>0</v>
+      </c>
+      <c r="C148" t="b">
+        <v>0</v>
+      </c>
+      <c r="D148" t="b">
+        <v>0</v>
+      </c>
+      <c r="E148" t="b">
+        <v>0</v>
+      </c>
+      <c r="F148" t="b">
+        <v>0</v>
+      </c>
+      <c r="G148" t="b">
+        <v>0</v>
+      </c>
+      <c r="H148" t="b">
+        <v>0</v>
+      </c>
+      <c r="I148" t="b">
+        <v>0</v>
+      </c>
+      <c r="J148" t="b">
+        <v>0</v>
+      </c>
+      <c r="K148" t="b">
+        <v>0</v>
+      </c>
+      <c r="L148" t="b">
+        <v>0</v>
+      </c>
+      <c r="M148" t="b">
+        <v>0</v>
+      </c>
+      <c r="N148" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14">
+      <c r="A149" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B149" t="b">
+        <v>0</v>
+      </c>
+      <c r="C149" t="b">
+        <v>0</v>
+      </c>
+      <c r="D149" t="b">
+        <v>0</v>
+      </c>
+      <c r="E149" t="b">
+        <v>0</v>
+      </c>
+      <c r="F149" t="b">
+        <v>0</v>
+      </c>
+      <c r="G149" t="b">
+        <v>0</v>
+      </c>
+      <c r="H149" t="b">
+        <v>0</v>
+      </c>
+      <c r="I149" t="b">
+        <v>0</v>
+      </c>
+      <c r="J149" t="b">
+        <v>0</v>
+      </c>
+      <c r="K149" t="b">
+        <v>0</v>
+      </c>
+      <c r="L149" t="b">
+        <v>0</v>
+      </c>
+      <c r="M149" t="b">
+        <v>0</v>
+      </c>
+      <c r="N149" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14">
+      <c r="A150" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B150" t="b">
+        <v>0</v>
+      </c>
+      <c r="C150" t="b">
+        <v>0</v>
+      </c>
+      <c r="D150" t="b">
+        <v>0</v>
+      </c>
+      <c r="E150" t="b">
+        <v>0</v>
+      </c>
+      <c r="F150" t="b">
+        <v>0</v>
+      </c>
+      <c r="G150" t="b">
+        <v>0</v>
+      </c>
+      <c r="H150" t="b">
+        <v>0</v>
+      </c>
+      <c r="I150" t="b">
+        <v>0</v>
+      </c>
+      <c r="J150" t="b">
+        <v>0</v>
+      </c>
+      <c r="K150" t="b">
+        <v>0</v>
+      </c>
+      <c r="L150" t="b">
+        <v>0</v>
+      </c>
+      <c r="M150" t="b">
+        <v>0</v>
+      </c>
+      <c r="N150" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14">
+      <c r="A151" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B151" t="b">
+        <v>0</v>
+      </c>
+      <c r="C151" t="b">
+        <v>0</v>
+      </c>
+      <c r="D151" t="b">
+        <v>0</v>
+      </c>
+      <c r="E151" t="b">
+        <v>0</v>
+      </c>
+      <c r="F151" t="b">
+        <v>0</v>
+      </c>
+      <c r="G151" t="b">
+        <v>0</v>
+      </c>
+      <c r="H151" t="b">
+        <v>0</v>
+      </c>
+      <c r="I151" t="b">
+        <v>0</v>
+      </c>
+      <c r="J151" t="b">
+        <v>0</v>
+      </c>
+      <c r="K151" t="b">
+        <v>0</v>
+      </c>
+      <c r="L151" t="b">
+        <v>0</v>
+      </c>
+      <c r="M151" t="b">
+        <v>0</v>
+      </c>
+      <c r="N151" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14">
+      <c r="A152" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B152" t="b">
+        <v>0</v>
+      </c>
+      <c r="C152" t="b">
+        <v>0</v>
+      </c>
+      <c r="D152" t="b">
+        <v>0</v>
+      </c>
+      <c r="E152" t="b">
+        <v>0</v>
+      </c>
+      <c r="F152" t="b">
+        <v>0</v>
+      </c>
+      <c r="G152" t="b">
+        <v>0</v>
+      </c>
+      <c r="H152" t="b">
+        <v>0</v>
+      </c>
+      <c r="I152" t="b">
+        <v>0</v>
+      </c>
+      <c r="J152" t="b">
+        <v>0</v>
+      </c>
+      <c r="K152" t="b">
+        <v>0</v>
+      </c>
+      <c r="L152" t="b">
+        <v>0</v>
+      </c>
+      <c r="M152" t="b">
+        <v>0</v>
+      </c>
+      <c r="N152" t="s">
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>